<commit_message>
Updated Quanto CDS Workbook
</commit_message>
<xml_diff>
--- a/Quanto CDS/Quanto CDS.xlsx
+++ b/Quanto CDS/Quanto CDS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26818"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nburg\Documents\MY_DOCUMENTS\QUANT\PAPERS\.QUANT_RESEARCH\Quanto CDS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9553D02B-FDA2-4874-9BA2-D2D4FDDD5DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650F5F77-5E2E-4FF7-8EFD-9D7B91950A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="38700" windowHeight="18555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="38700" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CDS" sheetId="1" r:id="rId1"/>
@@ -18704,7 +18704,7 @@
       </c>
       <c r="X3" s="49">
         <f t="shared" ref="X3:X44" si="4">IF(R3&gt;Maturity,"-",EXP(-QuantoHazardRate*R3))</f>
-        <v>0.99176552803828566</v>
+        <v>0.99169189218159381</v>
       </c>
       <c r="Y3" s="18">
         <f t="shared" ref="Y3:Y44" si="5">IF(R3&gt;Maturity,"-",EXP(-ZeroRate*R3))</f>
@@ -18716,7 +18716,7 @@
       </c>
       <c r="AA3" s="20">
         <f t="shared" ref="AA3:AA44" si="7">IF(R3&gt;Maturity,"-",Z3*EXP(-(QuantoHazardRate-DomesticHazardRate)*R3))</f>
-        <v>-4497.8461870524525</v>
+        <v>-4497.5122343712101</v>
       </c>
       <c r="AC3" s="16">
         <f>YearFraction</f>
@@ -18739,12 +18739,12 @@
         <v>-2325</v>
       </c>
       <c r="AH3" s="18">
-        <f t="shared" ref="AH3:AH44" si="12">IF(AC3&gt;Maturity,"-",1-EXP(-DomesticHazardRate*AC3))</f>
+        <f t="shared" ref="AH3" si="12">IF(AC3&gt;Maturity,"-",1-EXP(-DomesticHazardRate*AC3))</f>
         <v>7.4719451808615833E-3</v>
       </c>
       <c r="AI3" s="18">
-        <f t="shared" ref="AI3:AI44" si="13">IF(AC3&gt;Maturity,"-",1-EXP(-QuantoHazardRate*AC3))</f>
-        <v>8.2344719617143403E-3</v>
+        <f t="shared" ref="AI3" si="13">IF(AC3&gt;Maturity,"-",1-EXP(-QuantoHazardRate*AC3))</f>
+        <v>8.3081078184061852E-3</v>
       </c>
       <c r="AJ3" s="18">
         <f t="shared" ref="AJ3:AJ22" si="14">IF(AC3&gt;Maturity,"-",EXP(-ZeroRate*AC3))</f>
@@ -18756,7 +18756,7 @@
       </c>
       <c r="AL3" s="20">
         <f t="shared" ref="AL3:AL44" si="16">IF(AC3&gt;Maturity,"-",AK3/AH3*AI3)</f>
-        <v>-18.672451939647068</v>
+        <v>-18.839428280268059</v>
       </c>
       <c r="AN3" s="16">
         <f>YearFraction</f>
@@ -18771,12 +18771,12 @@
         <v>600000</v>
       </c>
       <c r="AQ3" s="18">
-        <f t="shared" ref="AQ3:AQ44" si="19">IF(AN3&gt;Maturity,"-",1-EXP(-DomesticHazardRate*AN3))</f>
+        <f t="shared" ref="AQ3" si="19">IF(AN3&gt;Maturity,"-",1-EXP(-DomesticHazardRate*AN3))</f>
         <v>7.4719451808615833E-3</v>
       </c>
       <c r="AR3" s="18">
-        <f t="shared" ref="AR3:AR44" si="20">IF(AN3&gt;Maturity,"-",1-EXP(-QuantoHazardRate*AN3))</f>
-        <v>8.2344719617143403E-3</v>
+        <f t="shared" ref="AR3" si="20">IF(AN3&gt;Maturity,"-",1-EXP(-QuantoHazardRate*AN3))</f>
+        <v>8.3081078184061852E-3</v>
       </c>
       <c r="AS3" s="18">
         <f t="shared" ref="AS3:AS22" si="21">IF(AN3&gt;Maturity,"-",EXP(-ZeroRate*AN3))</f>
@@ -18788,7 +18788,7 @@
       </c>
       <c r="AU3" s="20">
         <f t="shared" ref="AU3:AU44" si="23">IF(AN3&gt;Maturity,"-",AT3/AQ3*AR3)</f>
-        <v>4818.6972747476311</v>
+        <v>4861.787943294984</v>
       </c>
     </row>
     <row r="4" spans="2:48">
@@ -18838,7 +18838,7 @@
       </c>
       <c r="X4" s="50">
         <f t="shared" si="4"/>
-        <v>0.98359886260505958</v>
+        <v>0.98345280901870991</v>
       </c>
       <c r="Y4" s="23">
         <f t="shared" si="5"/>
@@ -18850,7 +18850,7 @@
       </c>
       <c r="AA4" s="25">
         <f t="shared" si="7"/>
-        <v>-4350.6710370714591</v>
+        <v>-4350.0250103911221</v>
       </c>
       <c r="AC4" s="21">
         <f t="shared" ref="AC4:AC10" si="26">AC3+YearFraction</f>
@@ -18873,12 +18873,12 @@
         <v>-2325</v>
       </c>
       <c r="AH4" s="23">
-        <f>IF(AC4&gt;Maturity,"-",EXP(-DomesticHazardRate*AC3)-EXP(-DomesticHazardRate*AC4))</f>
+        <f t="shared" ref="AH4:AH44" si="27">IF(AC4&gt;Maturity,"-",EXP(-DomesticHazardRate*AC3)-EXP(-DomesticHazardRate*AC4))</f>
         <v>7.4161152160757693E-3</v>
       </c>
       <c r="AI4" s="23">
-        <f>IF(AC4&gt;Maturity,"-",EXP(-QuantoHazardRate*AC3)-EXP(-QuantoHazardRate*AC4))</f>
-        <v>8.1666654332260835E-3</v>
+        <f t="shared" ref="AI4:AI44" si="28">IF(AC4&gt;Maturity,"-",EXP(-QuantoHazardRate*AC3)-EXP(-QuantoHazardRate*AC4))</f>
+        <v>8.239083162883909E-3</v>
       </c>
       <c r="AJ4" s="23">
         <f t="shared" si="14"/>
@@ -18890,10 +18890,10 @@
       </c>
       <c r="AL4" s="25">
         <f t="shared" si="16"/>
-        <v>-18.061465969819739</v>
+        <v>-18.221625629906331</v>
       </c>
       <c r="AN4" s="21">
-        <f t="shared" ref="AN4:AN10" si="27">AN3+YearFraction</f>
+        <f t="shared" ref="AN4:AN10" si="29">AN3+YearFraction</f>
         <v>0.5</v>
       </c>
       <c r="AO4" s="22">
@@ -18905,12 +18905,12 @@
         <v>600000</v>
       </c>
       <c r="AQ4" s="23">
-        <f>IF(AN4&gt;Maturity,"-",EXP(-DomesticHazardRate*AN3)-EXP(-DomesticHazardRate*AN4))</f>
+        <f t="shared" ref="AQ4:AQ44" si="30">IF(AN4&gt;Maturity,"-",EXP(-DomesticHazardRate*AN3)-EXP(-DomesticHazardRate*AN4))</f>
         <v>7.4161152160757693E-3</v>
       </c>
       <c r="AR4" s="23">
-        <f>IF(AN4&gt;Maturity,"-",EXP(-QuantoHazardRate*AN3)-EXP(-QuantoHazardRate*AN4))</f>
-        <v>8.1666654332260835E-3</v>
+        <f t="shared" ref="AR4:AR44" si="31">IF(AN4&gt;Maturity,"-",EXP(-QuantoHazardRate*AN3)-EXP(-QuantoHazardRate*AN4))</f>
+        <v>8.239083162883909E-3</v>
       </c>
       <c r="AS4" s="23">
         <f t="shared" si="21"/>
@@ -18922,7 +18922,7 @@
       </c>
       <c r="AU4" s="25">
         <f t="shared" si="23"/>
-        <v>4661.0234760825133</v>
+        <v>4702.3550012661508</v>
       </c>
     </row>
     <row r="5" spans="2:48">
@@ -18934,33 +18934,33 @@
       </c>
       <c r="H5" s="59">
         <f>E24</f>
-        <v>6666.1812065362392</v>
+        <v>7305.3674894290962</v>
       </c>
       <c r="I5" s="58">
         <v>0</v>
       </c>
       <c r="J5" s="58">
-        <f t="shared" ref="J5:O5" si="28">I5+5%</f>
+        <f t="shared" ref="J5:O5" si="32">I5+5%</f>
         <v>0.05</v>
       </c>
       <c r="K5" s="58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>0.1</v>
       </c>
       <c r="L5" s="58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>0.15000000000000002</v>
       </c>
       <c r="M5" s="58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>0.2</v>
       </c>
       <c r="N5" s="58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>0.25</v>
       </c>
       <c r="O5" s="58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>0.3</v>
       </c>
       <c r="P5" s="3"/>
@@ -18990,7 +18990,7 @@
       </c>
       <c r="X5" s="50">
         <f t="shared" si="4"/>
-        <v>0.97549944534936406</v>
+        <v>0.97528217704706799</v>
       </c>
       <c r="Y5" s="23">
         <f t="shared" si="5"/>
@@ -19002,7 +19002,7 @@
       </c>
       <c r="AA5" s="25">
         <f t="shared" si="7"/>
-        <v>-4208.3116419809467</v>
+        <v>-4207.3743449580261</v>
       </c>
       <c r="AC5" s="21">
         <f t="shared" si="26"/>
@@ -19025,12 +19025,12 @@
         <v>-2325</v>
       </c>
       <c r="AH5" s="23">
-        <f>IF(AC5&gt;Maturity,"-",EXP(-DomesticHazardRate*AC4)-EXP(-DomesticHazardRate*AC5))</f>
+        <f t="shared" si="27"/>
         <v>7.3607024097263052E-3</v>
       </c>
       <c r="AI5" s="23">
-        <f>IF(AC5&gt;Maturity,"-",EXP(-QuantoHazardRate*AC4)-EXP(-QuantoHazardRate*AC5))</f>
-        <v>8.099417255695518E-3</v>
+        <f t="shared" si="28"/>
+        <v>8.1706319716419173E-3</v>
       </c>
       <c r="AJ5" s="23">
         <f t="shared" si="14"/>
@@ -19042,10 +19042,10 @@
       </c>
       <c r="AL5" s="25">
         <f t="shared" si="16"/>
-        <v>-17.470472224716492</v>
+        <v>-17.624082623792766</v>
       </c>
       <c r="AN5" s="21">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>0.75</v>
       </c>
       <c r="AO5" s="22">
@@ -19057,12 +19057,12 @@
         <v>600000</v>
       </c>
       <c r="AQ5" s="23">
-        <f>IF(AN5&gt;Maturity,"-",EXP(-DomesticHazardRate*AN4)-EXP(-DomesticHazardRate*AN5))</f>
+        <f t="shared" si="30"/>
         <v>7.3607024097263052E-3</v>
       </c>
       <c r="AR5" s="23">
-        <f>IF(AN5&gt;Maturity,"-",EXP(-QuantoHazardRate*AN4)-EXP(-QuantoHazardRate*AN5))</f>
-        <v>8.099417255695518E-3</v>
+        <f t="shared" si="31"/>
+        <v>8.1706319716419173E-3</v>
       </c>
       <c r="AS5" s="23">
         <f t="shared" si="21"/>
@@ -19074,7 +19074,7 @@
       </c>
       <c r="AU5" s="25">
         <f t="shared" si="23"/>
-        <v>4508.5089612171596</v>
+        <v>4548.1503545271662</v>
       </c>
     </row>
     <row r="6" spans="2:48" ht="17.25">
@@ -19092,25 +19092,25 @@
       </c>
       <c r="I6" s="53">
         <f t="dataTable" ref="I6:O14" dt2D="1" dtr="1" r1="C15" r2="C16"/>
-        <v>490.9938538943461</v>
+        <v>2450.0495273290071</v>
       </c>
       <c r="J6" s="53">
-        <v>3776.0985597739273</v>
+        <v>5819.0876510507587</v>
       </c>
       <c r="K6" s="53">
-        <v>7039.1426896475823</v>
+        <v>9164.8358747583334</v>
       </c>
       <c r="L6" s="53">
-        <v>10280.282902775049</v>
+        <v>12487.464475857727</v>
       </c>
       <c r="M6" s="53">
-        <v>13499.674719701194</v>
+        <v>15787.142457408794</v>
       </c>
       <c r="N6" s="53">
-        <v>16697.472530630701</v>
+        <v>19064.037557776224</v>
       </c>
       <c r="O6" s="53">
-        <v>19873.829603741651</v>
+        <v>22318.316260206069</v>
       </c>
       <c r="P6" s="3"/>
       <c r="R6" s="35">
@@ -19139,7 +19139,7 @@
       </c>
       <c r="X6" s="50">
         <f t="shared" si="4"/>
-        <v>0.96746672251796684</v>
+        <v>0.96717942756679098</v>
       </c>
       <c r="Y6" s="23">
         <f t="shared" si="5"/>
@@ -19151,7 +19151,7 @@
       </c>
       <c r="AA6" s="25">
         <f t="shared" si="7"/>
-        <v>-4070.6104242607416</v>
+        <v>-4069.4016324792015</v>
       </c>
       <c r="AC6" s="21">
         <f t="shared" si="26"/>
@@ -19174,12 +19174,12 @@
         <v>-2325</v>
       </c>
       <c r="AH6" s="23">
-        <f>IF(AC6&gt;Maturity,"-",EXP(-DomesticHazardRate*AC5)-EXP(-DomesticHazardRate*AC6))</f>
+        <f t="shared" si="27"/>
         <v>7.3057036448281876E-3</v>
       </c>
       <c r="AI6" s="23">
-        <f>IF(AC6&gt;Maturity,"-",EXP(-QuantoHazardRate*AC5)-EXP(-QuantoHazardRate*AC6))</f>
-        <v>8.032722831397221E-3</v>
+        <f t="shared" si="28"/>
+        <v>8.102749480277005E-3</v>
       </c>
       <c r="AJ6" s="23">
         <f t="shared" si="14"/>
@@ -19191,10 +19191,10 @@
       </c>
       <c r="AL6" s="25">
         <f t="shared" si="16"/>
-        <v>-16.898816533751916</v>
+        <v>-17.046134886038082</v>
       </c>
       <c r="AN6" s="21">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>1</v>
       </c>
       <c r="AO6" s="22">
@@ -19206,12 +19206,12 @@
         <v>600000</v>
       </c>
       <c r="AQ6" s="23">
-        <f>IF(AN6&gt;Maturity,"-",EXP(-DomesticHazardRate*AN5)-EXP(-DomesticHazardRate*AN6))</f>
+        <f t="shared" si="30"/>
         <v>7.3057036448281876E-3</v>
       </c>
       <c r="AR6" s="23">
-        <f>IF(AN6&gt;Maturity,"-",EXP(-QuantoHazardRate*AN5)-EXP(-QuantoHazardRate*AN6))</f>
-        <v>8.032722831397221E-3</v>
+        <f t="shared" si="31"/>
+        <v>8.102749480277005E-3</v>
       </c>
       <c r="AS6" s="23">
         <f t="shared" si="21"/>
@@ -19223,7 +19223,7 @@
       </c>
       <c r="AU6" s="25">
         <f t="shared" si="23"/>
-        <v>4360.9849119359778</v>
+        <v>4399.0025512356351</v>
       </c>
     </row>
     <row r="7" spans="2:48">
@@ -19235,29 +19235,29 @@
       </c>
       <c r="G7" s="68"/>
       <c r="H7" s="57">
-        <f t="shared" ref="H7:H13" si="29">H6-0.25</f>
+        <f t="shared" ref="H7:H13" si="33">H6-0.25</f>
         <v>0.75</v>
       </c>
       <c r="I7" s="53">
-        <v>368.29158237140655</v>
+        <v>1838.6890888449489</v>
       </c>
       <c r="J7" s="53">
-        <v>3648.1257321535013</v>
+        <v>5181.5778540973915</v>
       </c>
       <c r="K7" s="53">
-        <v>6905.9752182797747</v>
+        <v>8501.5638489523044</v>
       </c>
       <c r="L7" s="53">
-        <v>10141.995872467327</v>
+        <v>11798.813018445966</v>
       </c>
       <c r="M7" s="53">
-        <v>13356.342395829874</v>
+        <v>15073.490076850918</v>
       </c>
       <c r="N7" s="53">
-        <v>16549.168367177474</v>
+        <v>18325.758516911963</v>
       </c>
       <c r="O7" s="53">
-        <v>19720.626251255548</v>
+        <v>21555.780619013465</v>
       </c>
       <c r="P7" s="3"/>
       <c r="R7" s="35">
@@ -19286,7 +19286,7 @@
       </c>
       <c r="X7" s="50">
         <f t="shared" si="4"/>
-        <v>0.95950014491750091</v>
+        <v>0.95914399660282179</v>
       </c>
       <c r="Y7" s="23">
         <f t="shared" si="5"/>
@@ -19298,7 +19298,7 @@
       </c>
       <c r="AA7" s="25">
         <f t="shared" si="7"/>
-        <v>-3937.4149625241171</v>
+        <v>-3935.9534685258895</v>
       </c>
       <c r="AC7" s="21">
         <f t="shared" si="26"/>
@@ -19321,12 +19321,12 @@
         <v>-2325</v>
       </c>
       <c r="AH7" s="23">
-        <f>IF(AC7&gt;Maturity,"-",EXP(-DomesticHazardRate*AC6)-EXP(-DomesticHazardRate*AC7))</f>
+        <f t="shared" si="27"/>
         <v>7.2511158276863386E-3</v>
       </c>
       <c r="AI7" s="23">
-        <f>IF(AC7&gt;Maturity,"-",EXP(-QuantoHazardRate*AC6)-EXP(-QuantoHazardRate*AC7))</f>
-        <v>7.9665776004659294E-3</v>
+        <f t="shared" si="28"/>
+        <v>8.0354309639691923E-3</v>
       </c>
       <c r="AJ7" s="23">
         <f t="shared" si="14"/>
@@ -19338,10 +19338,10 @@
       </c>
       <c r="AL7" s="25">
         <f t="shared" si="16"/>
-        <v>-16.345866131620578</v>
+        <v>-16.487139827676753</v>
       </c>
       <c r="AN7" s="21">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>1.25</v>
       </c>
       <c r="AO7" s="22">
@@ -19353,12 +19353,12 @@
         <v>600000</v>
       </c>
       <c r="AQ7" s="23">
-        <f>IF(AN7&gt;Maturity,"-",EXP(-DomesticHazardRate*AN6)-EXP(-DomesticHazardRate*AN7))</f>
+        <f t="shared" si="30"/>
         <v>7.2511158276863386E-3</v>
       </c>
       <c r="AR7" s="23">
-        <f>IF(AN7&gt;Maturity,"-",EXP(-QuantoHazardRate*AN6)-EXP(-QuantoHazardRate*AN7))</f>
-        <v>7.9665776004659294E-3</v>
+        <f t="shared" si="31"/>
+        <v>8.0354309639691923E-3</v>
       </c>
       <c r="AS7" s="23">
         <f t="shared" si="21"/>
@@ -19370,7 +19370,7 @@
       </c>
       <c r="AU7" s="25">
         <f t="shared" si="23"/>
-        <v>4218.2880339666008</v>
+        <v>4254.7457619810966</v>
       </c>
     </row>
     <row r="8" spans="2:48">
@@ -19382,29 +19382,29 @@
       </c>
       <c r="G8" s="68"/>
       <c r="H8" s="57">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0.5</v>
       </c>
       <c r="I8" s="53">
-        <v>245.55852166194381</v>
+        <v>1226.5613673771222</v>
       </c>
       <c r="J8" s="53">
-        <v>3520.1192001048257</v>
+        <v>4543.2282579866223</v>
       </c>
       <c r="K8" s="53">
-        <v>6772.7710183090749</v>
+        <v>7837.3768169795148</v>
       </c>
       <c r="L8" s="53">
-        <v>10003.668983204196</v>
+        <v>11109.168726918077</v>
       </c>
       <c r="M8" s="53">
-        <v>13212.966979185549</v>
+        <v>14358.764482087303</v>
       </c>
       <c r="N8" s="53">
-        <v>16400.817776339703</v>
+        <v>17586.323397331689</v>
       </c>
       <c r="O8" s="53">
-        <v>19567.373038609636</v>
+        <v>20792.003616825481</v>
       </c>
       <c r="P8" s="3"/>
       <c r="R8" s="35">
@@ -19433,7 +19433,7 @@
       </c>
       <c r="X8" s="50">
         <f t="shared" si="4"/>
-        <v>0.9515991678769169</v>
+        <v>0.95117532486566847</v>
       </c>
       <c r="Y8" s="23">
         <f t="shared" si="5"/>
@@ -19445,7 +19445,7 @@
       </c>
       <c r="AA8" s="25">
         <f t="shared" si="7"/>
-        <v>-3808.5778228026625</v>
+        <v>-3806.8814792711814</v>
       </c>
       <c r="AC8" s="21">
         <f t="shared" si="26"/>
@@ -19468,12 +19468,12 @@
         <v>-2325</v>
       </c>
       <c r="AH8" s="23">
-        <f>IF(AC8&gt;Maturity,"-",EXP(-DomesticHazardRate*AC7)-EXP(-DomesticHazardRate*AC8))</f>
+        <f t="shared" si="27"/>
         <v>7.1969358877218559E-3</v>
       </c>
       <c r="AI8" s="23">
-        <f>IF(AC8&gt;Maturity,"-",EXP(-QuantoHazardRate*AC7)-EXP(-QuantoHazardRate*AC8))</f>
-        <v>7.9009770405840118E-3</v>
+        <f t="shared" si="28"/>
+        <v>7.9686717371533211E-3</v>
       </c>
       <c r="AJ8" s="23">
         <f t="shared" si="14"/>
@@ -19485,10 +19485,10 @@
       </c>
       <c r="AL8" s="25">
         <f t="shared" si="16"/>
-        <v>-15.811008957887932</v>
+        <v>-15.946475932207823</v>
       </c>
       <c r="AN8" s="21">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>1.5</v>
       </c>
       <c r="AO8" s="22">
@@ -19500,12 +19500,12 @@
         <v>600000</v>
       </c>
       <c r="AQ8" s="23">
-        <f>IF(AN8&gt;Maturity,"-",EXP(-DomesticHazardRate*AN7)-EXP(-DomesticHazardRate*AN8))</f>
+        <f t="shared" si="30"/>
         <v>7.1969358877218559E-3</v>
       </c>
       <c r="AR8" s="23">
-        <f>IF(AN8&gt;Maturity,"-",EXP(-QuantoHazardRate*AN7)-EXP(-QuantoHazardRate*AN8))</f>
-        <v>7.9009770405840118E-3</v>
+        <f t="shared" si="31"/>
+        <v>7.9686717371533211E-3</v>
       </c>
       <c r="AS8" s="23">
         <f t="shared" si="21"/>
@@ -19517,7 +19517,7 @@
       </c>
       <c r="AU8" s="25">
         <f t="shared" si="23"/>
-        <v>4080.2603762291446</v>
+        <v>4115.2195954084718</v>
       </c>
     </row>
     <row r="9" spans="2:48">
@@ -19529,29 +19529,29 @@
       </c>
       <c r="G9" s="68"/>
       <c r="H9" s="57">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0.25</v>
       </c>
       <c r="I9" s="53">
-        <v>122.79466359566868</v>
+        <v>613.66534439889801</v>
       </c>
       <c r="J9" s="53">
-        <v>3392.0789542382336</v>
+        <v>3904.0376923530348</v>
       </c>
       <c r="K9" s="53">
-        <v>6639.5300790178226</v>
+        <v>7172.2734431269128</v>
       </c>
       <c r="L9" s="53">
-        <v>9865.3022228277769</v>
+        <v>10418.530086281353</v>
       </c>
       <c r="M9" s="53">
-        <v>13069.548456054712</v>
+        <v>13642.963964508446</v>
       </c>
       <c r="N9" s="53">
-        <v>16252.42074272973</v>
+        <v>16845.730282081982</v>
       </c>
       <c r="O9" s="53">
-        <v>19414.069948620199</v>
+        <v>20026.983113245551</v>
       </c>
       <c r="P9" s="3"/>
       <c r="R9" s="35">
@@ -19580,7 +19580,7 @@
       </c>
       <c r="X9" s="50">
         <f t="shared" si="4"/>
-        <v>0.94376325121024374</v>
+        <v>0.94327285771247693</v>
       </c>
       <c r="Y9" s="23">
         <f t="shared" si="5"/>
@@ -19592,7 +19592,7 @@
       </c>
       <c r="AA9" s="25">
         <f t="shared" si="7"/>
-        <v>-3683.9563953517163</v>
+        <v>-3682.0421565211409</v>
       </c>
       <c r="AC9" s="21">
         <f t="shared" si="26"/>
@@ -19615,12 +19615,12 @@
         <v>-2325</v>
       </c>
       <c r="AH9" s="23">
-        <f>IF(AC9&gt;Maturity,"-",EXP(-DomesticHazardRate*AC8)-EXP(-DomesticHazardRate*AC9))</f>
+        <f t="shared" si="27"/>
         <v>7.1431607772987071E-3</v>
       </c>
       <c r="AI9" s="23">
-        <f>IF(AC9&gt;Maturity,"-",EXP(-QuantoHazardRate*AC8)-EXP(-QuantoHazardRate*AC9))</f>
-        <v>7.8359166666731594E-3</v>
+        <f t="shared" si="28"/>
+        <v>7.9024671531915391E-3</v>
       </c>
       <c r="AJ9" s="23">
         <f t="shared" si="14"/>
@@ -19632,10 +19632,10 @@
       </c>
       <c r="AL9" s="25">
         <f t="shared" si="16"/>
-        <v>-15.293652979502856</v>
+        <v>-15.423542064561401</v>
       </c>
       <c r="AN9" s="21">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>1.75</v>
       </c>
       <c r="AO9" s="22">
@@ -19647,12 +19647,12 @@
         <v>600000</v>
       </c>
       <c r="AQ9" s="23">
-        <f>IF(AN9&gt;Maturity,"-",EXP(-DomesticHazardRate*AN8)-EXP(-DomesticHazardRate*AN9))</f>
+        <f t="shared" si="30"/>
         <v>7.1431607772987071E-3</v>
       </c>
       <c r="AR9" s="23">
-        <f>IF(AN9&gt;Maturity,"-",EXP(-QuantoHazardRate*AN8)-EXP(-QuantoHazardRate*AN9))</f>
-        <v>7.8359166666731594E-3</v>
+        <f t="shared" si="31"/>
+        <v>7.9024671531915391E-3</v>
       </c>
       <c r="AS9" s="23">
         <f t="shared" si="21"/>
@@ -19664,7 +19664,7 @@
       </c>
       <c r="AU9" s="25">
         <f t="shared" si="23"/>
-        <v>3946.749156000737</v>
+        <v>3980.2689198868134</v>
       </c>
     </row>
     <row r="10" spans="2:48">
@@ -19676,7 +19676,7 @@
       </c>
       <c r="G10" s="68"/>
       <c r="H10" s="57">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="I10" s="53">
@@ -19727,7 +19727,7 @@
       </c>
       <c r="X10" s="50">
         <f t="shared" si="4"/>
-        <v>0.93599185917965655</v>
+        <v>0.9354360451084256</v>
       </c>
       <c r="Y10" s="23">
         <f t="shared" si="5"/>
@@ -19739,7 +19739,7 @@
       </c>
       <c r="AA10" s="25">
         <f t="shared" si="7"/>
-        <v>-3563.4127367957453</v>
+        <v>-3561.2966981557829</v>
       </c>
       <c r="AC10" s="21">
         <f t="shared" si="26"/>
@@ -19762,12 +19762,12 @@
         <v>-2325</v>
       </c>
       <c r="AH10" s="23">
-        <f>IF(AC10&gt;Maturity,"-",EXP(-DomesticHazardRate*AC9)-EXP(-DomesticHazardRate*AC10))</f>
+        <f t="shared" si="27"/>
         <v>7.0897874715525333E-3</v>
       </c>
       <c r="AI10" s="23">
-        <f>IF(AC10&gt;Maturity,"-",EXP(-QuantoHazardRate*AC9)-EXP(-QuantoHazardRate*AC10))</f>
-        <v>7.7713920305871875E-3</v>
+        <f t="shared" si="28"/>
+        <v>7.8368126040513353E-3</v>
       </c>
       <c r="AJ10" s="23">
         <f t="shared" si="14"/>
@@ -19779,10 +19779,10 @@
       </c>
       <c r="AL10" s="25">
         <f t="shared" si="16"/>
-        <v>-14.793225535475484</v>
+        <v>-14.91775680273188</v>
       </c>
       <c r="AN10" s="21">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>2</v>
       </c>
       <c r="AO10" s="22">
@@ -19794,12 +19794,12 @@
         <v>600000</v>
       </c>
       <c r="AQ10" s="23">
-        <f>IF(AN10&gt;Maturity,"-",EXP(-DomesticHazardRate*AN9)-EXP(-DomesticHazardRate*AN10))</f>
+        <f t="shared" si="30"/>
         <v>7.0897874715525333E-3</v>
       </c>
       <c r="AR10" s="23">
-        <f>IF(AN10&gt;Maturity,"-",EXP(-QuantoHazardRate*AN9)-EXP(-QuantoHazardRate*AN10))</f>
-        <v>7.7713920305871875E-3</v>
+        <f t="shared" si="31"/>
+        <v>7.8368126040513353E-3</v>
       </c>
       <c r="AS10" s="23">
         <f t="shared" si="21"/>
@@ -19811,7 +19811,7 @@
       </c>
       <c r="AU10" s="25">
         <f t="shared" si="23"/>
-        <v>3817.6065898001248</v>
+        <v>3849.7436910275819</v>
       </c>
     </row>
     <row r="11" spans="2:48">
@@ -19825,33 +19825,33 @@
       <c r="F11" s="1"/>
       <c r="G11" s="68"/>
       <c r="H11" s="57">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>-0.25</v>
       </c>
       <c r="I11" s="53">
-        <v>-122.82547729997168</v>
+        <v>-614.43568711610715</v>
       </c>
       <c r="J11" s="53">
-        <v>3135.8972834793603</v>
+        <v>2623.1289627044825</v>
       </c>
       <c r="K11" s="53">
-        <v>6372.9379395869255</v>
+        <v>5839.3123169454702</v>
       </c>
       <c r="L11" s="53">
-        <v>9588.4490400848081</v>
+        <v>9034.263685873033</v>
       </c>
       <c r="M11" s="53">
-        <v>12782.582035457272</v>
+        <v>12208.131312535224</v>
       </c>
       <c r="N11" s="53">
-        <v>15955.487285615898</v>
+        <v>15361.062380480253</v>
       </c>
       <c r="O11" s="53">
-        <v>19107.314067845764</v>
+        <v>18493.203021418689</v>
       </c>
       <c r="P11" s="3"/>
       <c r="R11" s="35">
-        <f t="shared" ref="R11:R44" si="30">R10+YearFraction</f>
+        <f t="shared" ref="R11:R44" si="34">R10+YearFraction</f>
         <v>2.25</v>
       </c>
       <c r="S11" s="22">
@@ -19876,7 +19876,7 @@
       </c>
       <c r="X11" s="50">
         <f t="shared" si="4"/>
-        <v>0.92828446045884883</v>
+        <v>0.92766434158844124</v>
       </c>
       <c r="Y11" s="23">
         <f t="shared" si="5"/>
@@ -19888,10 +19888,10 @@
       </c>
       <c r="AA11" s="25">
         <f t="shared" si="7"/>
-        <v>-3446.8134174389006</v>
+        <v>-3444.5108538024579</v>
       </c>
       <c r="AC11" s="21">
-        <f t="shared" ref="AC11:AC44" si="31">AC10+YearFraction</f>
+        <f t="shared" ref="AC11:AC44" si="35">AC10+YearFraction</f>
         <v>2.25</v>
       </c>
       <c r="AD11" s="22">
@@ -19911,12 +19911,12 @@
         <v>-2325</v>
       </c>
       <c r="AH11" s="23">
-        <f>IF(AC11&gt;Maturity,"-",EXP(-DomesticHazardRate*AC10)-EXP(-DomesticHazardRate*AC11))</f>
+        <f t="shared" si="27"/>
         <v>7.0368129682212288E-3</v>
       </c>
       <c r="AI11" s="23">
-        <f>IF(AC11&gt;Maturity,"-",EXP(-QuantoHazardRate*AC10)-EXP(-QuantoHazardRate*AC11))</f>
-        <v>7.7073987208077233E-3</v>
+        <f t="shared" si="28"/>
+        <v>7.771703519984352E-3</v>
       </c>
       <c r="AJ11" s="23">
         <f t="shared" si="14"/>
@@ -19928,10 +19928,10 @@
       </c>
       <c r="AL11" s="25">
         <f t="shared" si="16"/>
-        <v>-14.309172702998817</v>
+        <v>-14.428557791325169</v>
       </c>
       <c r="AN11" s="21">
-        <f t="shared" ref="AN11:AN44" si="32">AN10+YearFraction</f>
+        <f t="shared" ref="AN11:AN44" si="36">AN10+YearFraction</f>
         <v>2.25</v>
       </c>
       <c r="AO11" s="22">
@@ -19943,12 +19943,12 @@
         <v>600000</v>
       </c>
       <c r="AQ11" s="23">
-        <f>IF(AN11&gt;Maturity,"-",EXP(-DomesticHazardRate*AN10)-EXP(-DomesticHazardRate*AN11))</f>
+        <f t="shared" si="30"/>
         <v>7.0368129682212288E-3</v>
       </c>
       <c r="AR11" s="23">
-        <f>IF(AN11&gt;Maturity,"-",EXP(-QuantoHazardRate*AN10)-EXP(-QuantoHazardRate*AN11))</f>
-        <v>7.7073987208077233E-3</v>
+        <f t="shared" si="31"/>
+        <v>7.771703519984352E-3</v>
       </c>
       <c r="AS11" s="23">
         <f t="shared" si="21"/>
@@ -19960,7 +19960,7 @@
       </c>
       <c r="AU11" s="25">
         <f t="shared" si="23"/>
-        <v>3692.6897298061458</v>
+        <v>3723.4987848581072</v>
       </c>
     </row>
     <row r="12" spans="2:48">
@@ -19974,33 +19974,33 @@
       <c r="F12" s="1"/>
       <c r="G12" s="68"/>
       <c r="H12" s="57">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>-0.5</v>
       </c>
       <c r="I12" s="53">
-        <v>-245.68177648117853</v>
+        <v>-1229.6427396335494</v>
       </c>
       <c r="J12" s="53">
-        <v>3007.755839794343</v>
+        <v>1981.408449600327</v>
       </c>
       <c r="K12" s="53">
-        <v>6239.5867179959241</v>
+        <v>5171.4518831969108</v>
       </c>
       <c r="L12" s="53">
-        <v>9449.9625933835414</v>
+        <v>8340.6328842662551</v>
       </c>
       <c r="M12" s="53">
-        <v>12639.034110541361</v>
+        <v>11489.095746976287</v>
       </c>
       <c r="N12" s="53">
-        <v>15806.950831310394</v>
+        <v>14616.98374392384</v>
       </c>
       <c r="O12" s="53">
-        <v>18953.861242662962</v>
+        <v>17724.439133453161</v>
       </c>
       <c r="P12" s="3"/>
       <c r="R12" s="35">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>2.5</v>
       </c>
       <c r="S12" s="22">
@@ -20025,7 +20025,7 @@
       </c>
       <c r="X12" s="50">
         <f t="shared" si="4"/>
-        <v>0.92064052809670527</v>
+        <v>0.91995720621923371</v>
       </c>
       <c r="Y12" s="23">
         <f t="shared" si="5"/>
@@ -20037,10 +20037,10 @@
       </c>
       <c r="AA12" s="25">
         <f t="shared" si="7"/>
-        <v>-3334.0293735717842</v>
+        <v>-3331.5547755701036</v>
       </c>
       <c r="AC12" s="21">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>2.5</v>
       </c>
       <c r="AD12" s="22">
@@ -20060,12 +20060,12 @@
         <v>-2325</v>
       </c>
       <c r="AH12" s="23">
-        <f>IF(AC12&gt;Maturity,"-",EXP(-DomesticHazardRate*AC11)-EXP(-DomesticHazardRate*AC12))</f>
+        <f t="shared" si="27"/>
         <v>6.9842342874746333E-3</v>
       </c>
       <c r="AI12" s="23">
-        <f>IF(AC12&gt;Maturity,"-",EXP(-QuantoHazardRate*AC11)-EXP(-QuantoHazardRate*AC12))</f>
-        <v>7.6439323621435573E-3</v>
+        <f t="shared" si="28"/>
+        <v>7.7071353692075295E-3</v>
       </c>
       <c r="AJ12" s="23">
         <f t="shared" si="14"/>
@@ -20077,10 +20077,10 @@
       </c>
       <c r="AL12" s="25">
         <f t="shared" si="16"/>
-        <v>-13.840958684313744</v>
+        <v>-13.955401116304536</v>
       </c>
       <c r="AN12" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>2.5</v>
       </c>
       <c r="AO12" s="22">
@@ -20092,12 +20092,12 @@
         <v>600000</v>
       </c>
       <c r="AQ12" s="23">
-        <f>IF(AN12&gt;Maturity,"-",EXP(-DomesticHazardRate*AN11)-EXP(-DomesticHazardRate*AN12))</f>
+        <f t="shared" si="30"/>
         <v>6.9842342874746333E-3</v>
       </c>
       <c r="AR12" s="23">
-        <f>IF(AN12&gt;Maturity,"-",EXP(-QuantoHazardRate*AN11)-EXP(-QuantoHazardRate*AN12))</f>
-        <v>7.6439323621435573E-3</v>
+        <f t="shared" si="31"/>
+        <v>7.7071353692075295E-3</v>
       </c>
       <c r="AS12" s="23">
         <f t="shared" si="21"/>
@@ -20109,7 +20109,7 @@
       </c>
       <c r="AU12" s="25">
         <f t="shared" si="23"/>
-        <v>3571.8603056293532</v>
+        <v>3601.3938364656869</v>
       </c>
     </row>
     <row r="13" spans="2:48">
@@ -20117,33 +20117,33 @@
       <c r="F13" s="1"/>
       <c r="G13" s="68"/>
       <c r="H13" s="57">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>-0.75</v>
       </c>
       <c r="I13" s="53">
-        <v>-368.56890572292468</v>
+        <v>-1845.6221816261532</v>
       </c>
       <c r="J13" s="53">
-        <v>2879.5806447060095</v>
+        <v>1338.8422687901257</v>
       </c>
       <c r="K13" s="53">
-        <v>6106.1987141816862</v>
+        <v>4502.6697447231345</v>
       </c>
       <c r="L13" s="53">
-        <v>9311.4362268996701</v>
+        <v>7646.0016498733385</v>
       </c>
       <c r="M13" s="53">
-        <v>12495.44302424034</v>
+        <v>10768.978396263883</v>
       </c>
       <c r="N13" s="53">
-        <v>15658.367872629409</v>
+        <v>13871.739411277922</v>
       </c>
       <c r="O13" s="53">
-        <v>18800.358471341249</v>
+        <v>16954.423144645094</v>
       </c>
       <c r="P13" s="3"/>
       <c r="R13" s="35">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>2.75</v>
       </c>
       <c r="S13" s="22">
@@ -20168,7 +20168,7 @@
       </c>
       <c r="X13" s="50">
         <f t="shared" si="4"/>
-        <v>0.91305953948127505</v>
+        <v>0.91231410256164458</v>
       </c>
       <c r="Y13" s="23">
         <f t="shared" si="5"/>
@@ -20180,10 +20180,10 @@
       </c>
       <c r="AA13" s="25">
         <f t="shared" si="7"/>
-        <v>-3224.9357646109083</v>
+        <v>-3222.3028736783599</v>
       </c>
       <c r="AC13" s="21">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>2.75</v>
       </c>
       <c r="AD13" s="22">
@@ -20203,12 +20203,12 @@
         <v>-2325</v>
       </c>
       <c r="AH13" s="23">
-        <f>IF(AC13&gt;Maturity,"-",EXP(-DomesticHazardRate*AC12)-EXP(-DomesticHazardRate*AC13))</f>
+        <f t="shared" si="27"/>
         <v>6.9320484717483311E-3</v>
       </c>
       <c r="AI13" s="23">
-        <f>IF(AC13&gt;Maturity,"-",EXP(-QuantoHazardRate*AC12)-EXP(-QuantoHazardRate*AC13))</f>
-        <v>7.5809886154302175E-3</v>
+        <f t="shared" si="28"/>
+        <v>7.6431036575891342E-3</v>
       </c>
       <c r="AJ13" s="23">
         <f t="shared" si="14"/>
@@ -20220,10 +20220,10 @@
       </c>
       <c r="AL13" s="25">
         <f t="shared" si="16"/>
-        <v>-13.388065213632448</v>
+        <v>-13.49776070024464</v>
       </c>
       <c r="AN13" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>2.75</v>
       </c>
       <c r="AO13" s="22">
@@ -20235,12 +20235,12 @@
         <v>600000</v>
       </c>
       <c r="AQ13" s="23">
-        <f>IF(AN13&gt;Maturity,"-",EXP(-DomesticHazardRate*AN12)-EXP(-DomesticHazardRate*AN13))</f>
+        <f t="shared" si="30"/>
         <v>6.9320484717483311E-3</v>
       </c>
       <c r="AR13" s="23">
-        <f>IF(AN13&gt;Maturity,"-",EXP(-QuantoHazardRate*AN12)-EXP(-QuantoHazardRate*AN13))</f>
-        <v>7.5809886154302175E-3</v>
+        <f t="shared" si="31"/>
+        <v>7.6431036575891342E-3</v>
       </c>
       <c r="AS13" s="23">
         <f t="shared" si="21"/>
@@ -20252,7 +20252,7 @@
       </c>
       <c r="AU13" s="25">
         <f t="shared" si="23"/>
-        <v>3454.9845712599863</v>
+        <v>3483.2930839341002</v>
       </c>
     </row>
     <row r="14" spans="2:48">
@@ -20267,29 +20267,29 @@
         <v>-1</v>
       </c>
       <c r="I14" s="53">
-        <v>-491.48687320666795</v>
+        <v>-2462.3750385594758</v>
       </c>
       <c r="J14" s="53">
-        <v>2751.3716888113195</v>
+        <v>695.4292415356249</v>
       </c>
       <c r="K14" s="53">
-        <v>5972.7739174105009</v>
+        <v>3832.9645557994736</v>
       </c>
       <c r="L14" s="53">
-        <v>9172.8699284563845</v>
+        <v>6950.3684558290624</v>
       </c>
       <c r="M14" s="53">
-        <v>12351.808762818422</v>
+        <v>10047.777537815309</v>
       </c>
       <c r="N14" s="53">
-        <v>15509.73839415906</v>
+        <v>13125.327449257857</v>
       </c>
       <c r="O14" s="53">
-        <v>18646.805736666494</v>
+        <v>16183.152895631916</v>
       </c>
       <c r="P14" s="3"/>
       <c r="R14" s="35">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>3</v>
       </c>
       <c r="S14" s="22">
@@ -20314,7 +20314,7 @@
       </c>
       <c r="X14" s="50">
         <f t="shared" si="4"/>
-        <v>0.90554097630404062</v>
+        <v>0.90473449863331001</v>
       </c>
       <c r="Y14" s="23">
         <f t="shared" si="5"/>
@@ -20326,10 +20326,10 @@
       </c>
       <c r="AA14" s="25">
         <f t="shared" si="7"/>
-        <v>-3119.4118349127448</v>
+        <v>-3116.6336768210608</v>
       </c>
       <c r="AC14" s="21">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>3</v>
       </c>
       <c r="AD14" s="22">
@@ -20349,12 +20349,12 @@
         <v>-2325</v>
       </c>
       <c r="AH14" s="23">
-        <f>IF(AC14&gt;Maturity,"-",EXP(-DomesticHazardRate*AC13)-EXP(-DomesticHazardRate*AC14))</f>
+        <f t="shared" si="27"/>
         <v>6.8802525855763408E-3</v>
       </c>
       <c r="AI14" s="23">
-        <f>IF(AC14&gt;Maturity,"-",EXP(-QuantoHazardRate*AC13)-EXP(-QuantoHazardRate*AC14))</f>
-        <v>7.5185631772344275E-3</v>
+        <f t="shared" si="28"/>
+        <v>7.5796039283345662E-3</v>
       </c>
       <c r="AJ14" s="23">
         <f t="shared" si="14"/>
@@ -20366,10 +20366,10 @@
       </c>
       <c r="AL14" s="25">
         <f t="shared" si="16"/>
-        <v>-12.949990983472398</v>
+        <v>-13.055127717411761</v>
       </c>
       <c r="AN14" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>3</v>
       </c>
       <c r="AO14" s="22">
@@ -20381,12 +20381,12 @@
         <v>600000</v>
       </c>
       <c r="AQ14" s="23">
-        <f>IF(AN14&gt;Maturity,"-",EXP(-DomesticHazardRate*AN13)-EXP(-DomesticHazardRate*AN14))</f>
+        <f t="shared" si="30"/>
         <v>6.8802525855763408E-3</v>
       </c>
       <c r="AR14" s="23">
-        <f>IF(AN14&gt;Maturity,"-",EXP(-QuantoHazardRate*AN13)-EXP(-QuantoHazardRate*AN14))</f>
-        <v>7.5185631772344275E-3</v>
+        <f t="shared" si="31"/>
+        <v>7.5796039283345662E-3</v>
       </c>
       <c r="AS14" s="23">
         <f t="shared" si="21"/>
@@ -20398,7 +20398,7 @@
       </c>
       <c r="AU14" s="25">
         <f t="shared" si="23"/>
-        <v>3341.9331570251352</v>
+        <v>3369.0652173965836</v>
       </c>
     </row>
     <row r="15" spans="2:48" ht="18">
@@ -20415,36 +20415,36 @@
         <v>47</v>
       </c>
       <c r="I15" s="65">
-        <f t="shared" ref="I15:O15" si="33">I6-I14</f>
-        <v>982.48072710101405</v>
+        <f t="shared" ref="I15:O15" si="37">I6-I14</f>
+        <v>4912.4245658884829</v>
       </c>
       <c r="J15" s="65">
-        <f t="shared" si="33"/>
-        <v>1024.7268709626078</v>
+        <f t="shared" si="37"/>
+        <v>5123.6584095151338</v>
       </c>
       <c r="K15" s="65">
-        <f t="shared" si="33"/>
-        <v>1066.3687722370814</v>
+        <f t="shared" si="37"/>
+        <v>5331.8713189588598</v>
       </c>
       <c r="L15" s="65">
-        <f t="shared" si="33"/>
-        <v>1107.4129743186641</v>
+        <f t="shared" si="37"/>
+        <v>5537.0960200286645</v>
       </c>
       <c r="M15" s="65">
-        <f t="shared" si="33"/>
-        <v>1147.8659568827716</v>
+        <f t="shared" si="37"/>
+        <v>5739.364919593485</v>
       </c>
       <c r="N15" s="65">
-        <f t="shared" si="33"/>
-        <v>1187.7341364716412</v>
+        <f t="shared" si="37"/>
+        <v>5938.7101085183676</v>
       </c>
       <c r="O15" s="65">
-        <f t="shared" si="33"/>
-        <v>1227.0238670751569</v>
+        <f t="shared" si="37"/>
+        <v>6135.1633645741531</v>
       </c>
       <c r="P15" s="3"/>
       <c r="R15" s="35">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>3.25</v>
       </c>
       <c r="S15" s="22">
@@ -20469,7 +20469,7 @@
       </c>
       <c r="X15" s="50">
         <f t="shared" si="4"/>
-        <v>0.89808432452448161</v>
+        <v>0.89721786687163274</v>
       </c>
       <c r="Y15" s="23">
         <f t="shared" si="5"/>
@@ -20481,10 +20481,10 @@
       </c>
       <c r="AA15" s="25">
         <f t="shared" si="7"/>
-        <v>-3017.3407801093726</v>
+        <v>-3014.4296971088283</v>
       </c>
       <c r="AC15" s="21">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>3.25</v>
       </c>
       <c r="AD15" s="22">
@@ -20504,12 +20504,12 @@
         <v>-2325</v>
       </c>
       <c r="AH15" s="23">
-        <f>IF(AC15&gt;Maturity,"-",EXP(-DomesticHazardRate*AC14)-EXP(-DomesticHazardRate*AC15))</f>
+        <f t="shared" si="27"/>
         <v>6.8288437154264692E-3</v>
       </c>
       <c r="AI15" s="23">
-        <f>IF(AC15&gt;Maturity,"-",EXP(-QuantoHazardRate*AC14)-EXP(-QuantoHazardRate*AC15))</f>
-        <v>7.4566517795590093E-3</v>
+        <f t="shared" si="28"/>
+        <v>7.5166317616772726E-3</v>
       </c>
       <c r="AJ15" s="23">
         <f t="shared" si="14"/>
@@ -20521,10 +20521,10 @@
       </c>
       <c r="AL15" s="25">
         <f t="shared" si="16"/>
-        <v>-12.526251089757885</v>
+        <v>-12.627010028029908</v>
       </c>
       <c r="AN15" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>3.25</v>
       </c>
       <c r="AO15" s="22">
@@ -20536,12 +20536,12 @@
         <v>600000</v>
       </c>
       <c r="AQ15" s="23">
-        <f>IF(AN15&gt;Maturity,"-",EXP(-DomesticHazardRate*AN14)-EXP(-DomesticHazardRate*AN15))</f>
+        <f t="shared" si="30"/>
         <v>6.8288437154264692E-3</v>
       </c>
       <c r="AR15" s="23">
-        <f>IF(AN15&gt;Maturity,"-",EXP(-QuantoHazardRate*AN14)-EXP(-QuantoHazardRate*AN15))</f>
-        <v>7.4566517795590093E-3</v>
+        <f t="shared" si="31"/>
+        <v>7.5166317616772726E-3</v>
       </c>
       <c r="AS15" s="23">
         <f t="shared" si="21"/>
@@ -20553,7 +20553,7 @@
       </c>
       <c r="AU15" s="25">
         <f t="shared" si="23"/>
-        <v>3232.5809263891315</v>
+        <v>3258.5832330399762</v>
       </c>
     </row>
     <row r="16" spans="2:48" ht="18">
@@ -20568,7 +20568,7 @@
       <c r="G16" s="1"/>
       <c r="P16" s="3"/>
       <c r="R16" s="35">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>3.5</v>
       </c>
       <c r="S16" s="22">
@@ -20593,7 +20593,7 @@
       </c>
       <c r="X16" s="50">
         <f t="shared" si="4"/>
-        <v>0.8906890743349295</v>
+        <v>0.88976368409706286</v>
       </c>
       <c r="Y16" s="23">
         <f t="shared" si="5"/>
@@ -20605,10 +20605,10 @@
       </c>
       <c r="AA16" s="25">
         <f t="shared" si="7"/>
-        <v>-2918.6096178178095</v>
+        <v>-2915.5772994406148</v>
       </c>
       <c r="AC16" s="21">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>3.5</v>
       </c>
       <c r="AD16" s="22">
@@ -20628,12 +20628,12 @@
         <v>-2325</v>
       </c>
       <c r="AH16" s="23">
-        <f>IF(AC16&gt;Maturity,"-",EXP(-DomesticHazardRate*AC15)-EXP(-DomesticHazardRate*AC16))</f>
+        <f t="shared" si="27"/>
         <v>6.7778189695361091E-3</v>
       </c>
       <c r="AI16" s="23">
-        <f>IF(AC16&gt;Maturity,"-",EXP(-QuantoHazardRate*AC15)-EXP(-QuantoHazardRate*AC16))</f>
-        <v>7.3952501895521161E-3</v>
+        <f t="shared" si="28"/>
+        <v>7.4541827745698841E-3</v>
       </c>
       <c r="AJ16" s="23">
         <f t="shared" si="14"/>
@@ -20645,10 +20645,10 @@
       </c>
       <c r="AL16" s="25">
         <f t="shared" si="16"/>
-        <v>-12.116376495081782</v>
+        <v>-12.212931631094962</v>
       </c>
       <c r="AN16" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>3.5</v>
       </c>
       <c r="AO16" s="22">
@@ -20660,12 +20660,12 @@
         <v>600000</v>
       </c>
       <c r="AQ16" s="23">
-        <f>IF(AN16&gt;Maturity,"-",EXP(-DomesticHazardRate*AN15)-EXP(-DomesticHazardRate*AN16))</f>
+        <f t="shared" si="30"/>
         <v>6.7778189695361091E-3</v>
       </c>
       <c r="AR16" s="23">
-        <f>IF(AN16&gt;Maturity,"-",EXP(-QuantoHazardRate*AN15)-EXP(-QuantoHazardRate*AN16))</f>
-        <v>7.3952501895521161E-3</v>
+        <f t="shared" si="31"/>
+        <v>7.4541827745698841E-3</v>
       </c>
       <c r="AS16" s="23">
         <f t="shared" si="21"/>
@@ -20677,7 +20677,7 @@
       </c>
       <c r="AU16" s="25">
         <f t="shared" si="23"/>
-        <v>3126.8068374404602</v>
+        <v>3151.7242918954744</v>
       </c>
     </row>
     <row r="17" spans="2:47" ht="18">
@@ -20692,7 +20692,7 @@
       <c r="G17" s="1"/>
       <c r="P17" s="3"/>
       <c r="R17" s="35">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>3.75</v>
       </c>
       <c r="S17" s="22">
@@ -20717,7 +20717,7 @@
       </c>
       <c r="X17" s="50">
         <f t="shared" si="4"/>
-        <v>0.88335472012571326</v>
+        <v>0.88237143147668207</v>
       </c>
       <c r="Y17" s="23">
         <f t="shared" si="5"/>
@@ -20729,10 +20729,10 @@
       </c>
       <c r="AA17" s="25">
         <f t="shared" si="7"/>
-        <v>-2823.109062579882</v>
+        <v>-2819.9665751589546</v>
       </c>
       <c r="AC17" s="21">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>3.75</v>
       </c>
       <c r="AD17" s="22">
@@ -20752,12 +20752,12 @@
         <v>-2325</v>
       </c>
       <c r="AH17" s="23">
-        <f>IF(AC17&gt;Maturity,"-",EXP(-DomesticHazardRate*AC16)-EXP(-DomesticHazardRate*AC17))</f>
+        <f t="shared" si="27"/>
         <v>6.7271754777499249E-3</v>
       </c>
       <c r="AI17" s="23">
-        <f>IF(AC17&gt;Maturity,"-",EXP(-QuantoHazardRate*AC16)-EXP(-QuantoHazardRate*AC17))</f>
-        <v>7.3343542092162428E-3</v>
+        <f t="shared" si="28"/>
+        <v>7.3922526203807903E-3</v>
       </c>
       <c r="AJ17" s="23">
         <f t="shared" si="14"/>
@@ -20769,10 +20769,10 @@
       </c>
       <c r="AL17" s="25">
         <f t="shared" si="16"/>
-        <v>-11.7199135095257</v>
+        <v>-11.812432135137589</v>
       </c>
       <c r="AN17" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>3.75</v>
       </c>
       <c r="AO17" s="22">
@@ -20784,12 +20784,12 @@
         <v>600000</v>
       </c>
       <c r="AQ17" s="23">
-        <f>IF(AN17&gt;Maturity,"-",EXP(-DomesticHazardRate*AN16)-EXP(-DomesticHazardRate*AN17))</f>
+        <f t="shared" si="30"/>
         <v>6.7271754777499249E-3</v>
       </c>
       <c r="AR17" s="23">
-        <f>IF(AN17&gt;Maturity,"-",EXP(-QuantoHazardRate*AN16)-EXP(-QuantoHazardRate*AN17))</f>
-        <v>7.3343542092162428E-3</v>
+        <f t="shared" si="31"/>
+        <v>7.3922526203807903E-3</v>
       </c>
       <c r="AS17" s="23">
         <f t="shared" si="21"/>
@@ -20801,7 +20801,7 @@
       </c>
       <c r="AU17" s="25">
         <f t="shared" si="23"/>
-        <v>3024.4938089098578</v>
+        <v>3048.3695832613125</v>
       </c>
     </row>
     <row r="18" spans="2:47" ht="18">
@@ -20816,7 +20816,7 @@
       <c r="G18" s="1"/>
       <c r="P18" s="3"/>
       <c r="R18" s="35">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>4</v>
       </c>
       <c r="S18" s="22">
@@ -20841,7 +20841,7 @@
       </c>
       <c r="X18" s="50">
         <f t="shared" si="4"/>
-        <v>0.87608076045059002</v>
+        <v>0.87504059448809246</v>
       </c>
       <c r="Y18" s="23">
         <f t="shared" si="5"/>
@@ -20853,10 +20853,10 @@
       </c>
       <c r="AA18" s="25">
         <f t="shared" si="7"/>
-        <v>-2730.7334048942248</v>
+        <v>-2727.4912198484476</v>
       </c>
       <c r="AC18" s="21">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>4</v>
       </c>
       <c r="AD18" s="22">
@@ -20876,12 +20876,12 @@
         <v>-2325</v>
       </c>
       <c r="AH18" s="23">
-        <f>IF(AC18&gt;Maturity,"-",EXP(-DomesticHazardRate*AC17)-EXP(-DomesticHazardRate*AC18))</f>
+        <f t="shared" si="27"/>
         <v>6.676910391358204E-3</v>
       </c>
       <c r="AI18" s="23">
-        <f>IF(AC18&gt;Maturity,"-",EXP(-QuantoHazardRate*AC17)-EXP(-QuantoHazardRate*AC18))</f>
-        <v>7.2739596751232316E-3</v>
+        <f t="shared" si="28"/>
+        <v>7.3308369885896063E-3</v>
       </c>
       <c r="AJ18" s="23">
         <f t="shared" si="14"/>
@@ -20893,10 +20893,10 @@
       </c>
       <c r="AL18" s="25">
         <f t="shared" si="16"/>
-        <v>-11.336423288474226</v>
+        <v>-11.425066246335431</v>
       </c>
       <c r="AN18" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>4</v>
       </c>
       <c r="AO18" s="22">
@@ -20908,12 +20908,12 @@
         <v>600000</v>
       </c>
       <c r="AQ18" s="23">
-        <f>IF(AN18&gt;Maturity,"-",EXP(-DomesticHazardRate*AN17)-EXP(-DomesticHazardRate*AN18))</f>
+        <f t="shared" si="30"/>
         <v>6.676910391358204E-3</v>
       </c>
       <c r="AR18" s="23">
-        <f>IF(AN18&gt;Maturity,"-",EXP(-QuantoHazardRate*AN17)-EXP(-QuantoHazardRate*AN18))</f>
-        <v>7.2739596751232316E-3</v>
+        <f t="shared" si="31"/>
+        <v>7.3308369885896063E-3</v>
       </c>
       <c r="AS18" s="23">
         <f t="shared" si="21"/>
@@ -20925,7 +20925,7 @@
       </c>
       <c r="AU18" s="25">
         <f t="shared" si="23"/>
-        <v>2925.5285905739934</v>
+        <v>2948.4041926026916</v>
       </c>
     </row>
     <row r="19" spans="2:47" ht="17.25">
@@ -20933,15 +20933,15 @@
         <v>33</v>
       </c>
       <c r="C19" s="60">
-        <f>(1+FX_Jump)*(1+0.5*Correlation*Volatility_Credit*Volatility_FX)*DomesticHazardRate</f>
-        <v>3.3074249999999999E-2</v>
+        <f>(1+FX_Jump)*(1+0.5*Correlation*Volatility_Credit*Volatility_FX*Maturity)*DomesticHazardRate</f>
+        <v>3.3371250000000005E-2</v>
       </c>
       <c r="E19" s="66"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="P19" s="3"/>
       <c r="R19" s="35">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>4.25</v>
       </c>
       <c r="S19" s="22">
@@ -20966,7 +20966,7 @@
       </c>
       <c r="X19" s="50">
         <f t="shared" si="4"/>
-        <v>0.8688666979924623</v>
+        <v>0.86777066288360305</v>
       </c>
       <c r="Y19" s="23">
         <f t="shared" si="5"/>
@@ -20978,10 +20978,10 @@
       </c>
       <c r="AA19" s="25">
         <f t="shared" si="7"/>
-        <v>-2641.380394206506</v>
+        <v>-2638.0484151416026</v>
       </c>
       <c r="AC19" s="21">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>4.25</v>
       </c>
       <c r="AD19" s="22">
@@ -21001,12 +21001,12 @@
         <v>-2325</v>
       </c>
       <c r="AH19" s="23">
-        <f>IF(AC19&gt;Maturity,"-",EXP(-DomesticHazardRate*AC18)-EXP(-DomesticHazardRate*AC19))</f>
+        <f t="shared" si="27"/>
         <v>6.6270208829363186E-3</v>
       </c>
       <c r="AI19" s="23">
-        <f>IF(AC19&gt;Maturity,"-",EXP(-QuantoHazardRate*AC18)-EXP(-QuantoHazardRate*AC19))</f>
-        <v>7.2140624581277235E-3</v>
+        <f t="shared" si="28"/>
+        <v>7.2699316044894102E-3</v>
       </c>
       <c r="AJ19" s="23">
         <f t="shared" si="14"/>
@@ -21018,10 +21018,10 @@
       </c>
       <c r="AL19" s="25">
         <f t="shared" si="16"/>
-        <v>-10.965481346855043</v>
+        <v>-11.050403273418565</v>
       </c>
       <c r="AN19" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>4.25</v>
       </c>
       <c r="AO19" s="22">
@@ -21033,12 +21033,12 @@
         <v>600000</v>
       </c>
       <c r="AQ19" s="23">
-        <f>IF(AN19&gt;Maturity,"-",EXP(-DomesticHazardRate*AN18)-EXP(-DomesticHazardRate*AN19))</f>
+        <f t="shared" si="30"/>
         <v>6.6270208829363186E-3</v>
       </c>
       <c r="AR19" s="23">
-        <f>IF(AN19&gt;Maturity,"-",EXP(-QuantoHazardRate*AN18)-EXP(-QuantoHazardRate*AN19))</f>
-        <v>7.2140624581277235E-3</v>
+        <f t="shared" si="31"/>
+        <v>7.2699316044894102E-3</v>
       </c>
       <c r="AS19" s="23">
         <f t="shared" si="21"/>
@@ -21050,13 +21050,13 @@
       </c>
       <c r="AU19" s="25">
         <f t="shared" si="23"/>
-        <v>2829.801637898076</v>
+        <v>2851.7169737854365</v>
       </c>
     </row>
     <row r="20" spans="2:47">
       <c r="P20" s="3"/>
       <c r="R20" s="35">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>4.5</v>
       </c>
       <c r="S20" s="22">
@@ -21081,7 +21081,7 @@
       </c>
       <c r="X20" s="50">
         <f t="shared" si="4"/>
-        <v>0.86171203952937603</v>
+        <v>0.86056113065471629</v>
       </c>
       <c r="Y20" s="23">
         <f t="shared" si="5"/>
@@ -21093,10 +21093,10 @@
       </c>
       <c r="AA20" s="25">
         <f t="shared" si="7"/>
-        <v>-2554.9511257283516</v>
+        <v>-2551.5387144006318</v>
       </c>
       <c r="AC20" s="21">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>4.5</v>
       </c>
       <c r="AD20" s="22">
@@ -21116,12 +21116,12 @@
         <v>-2325</v>
       </c>
       <c r="AH20" s="23">
-        <f>IF(AC20&gt;Maturity,"-",EXP(-DomesticHazardRate*AC19)-EXP(-DomesticHazardRate*AC20))</f>
+        <f t="shared" si="27"/>
         <v>6.5775041461867412E-3</v>
       </c>
       <c r="AI20" s="23">
-        <f>IF(AC20&gt;Maturity,"-",EXP(-QuantoHazardRate*AC19)-EXP(-QuantoHazardRate*AC20))</f>
-        <v>7.154658463086272E-3</v>
+        <f t="shared" si="28"/>
+        <v>7.2095322288867614E-3</v>
       </c>
       <c r="AJ20" s="23">
         <f t="shared" si="14"/>
@@ -21133,10 +21133,10 @@
       </c>
       <c r="AL20" s="25">
         <f t="shared" si="16"/>
-        <v>-10.606677089278955</v>
+        <v>-10.688026648803206</v>
       </c>
       <c r="AN20" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>4.5</v>
       </c>
       <c r="AO20" s="22">
@@ -21148,12 +21148,12 @@
         <v>600000</v>
       </c>
       <c r="AQ20" s="23">
-        <f>IF(AN20&gt;Maturity,"-",EXP(-DomesticHazardRate*AN19)-EXP(-DomesticHazardRate*AN20))</f>
+        <f t="shared" si="30"/>
         <v>6.5775041461867412E-3</v>
       </c>
       <c r="AR20" s="23">
-        <f>IF(AN20&gt;Maturity,"-",EXP(-QuantoHazardRate*AN19)-EXP(-QuantoHazardRate*AN20))</f>
-        <v>7.154658463086272E-3</v>
+        <f t="shared" si="31"/>
+        <v>7.2095322288867614E-3</v>
       </c>
       <c r="AS20" s="23">
         <f t="shared" si="21"/>
@@ -21165,13 +21165,13 @@
       </c>
       <c r="AU20" s="25">
         <f t="shared" si="23"/>
-        <v>2737.2069907816663</v>
+        <v>2758.2004254976018</v>
       </c>
     </row>
     <row r="21" spans="2:47">
       <c r="P21" s="3"/>
       <c r="R21" s="35">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>4.75</v>
       </c>
       <c r="S21" s="22">
@@ -21196,7 +21196,7 @@
       </c>
       <c r="X21" s="50">
         <f t="shared" si="4"/>
-        <v>0.85461629590079957</v>
+        <v>0.85341149599690735</v>
       </c>
       <c r="Y21" s="23">
         <f t="shared" si="5"/>
@@ -21208,10 +21208,10 @@
       </c>
       <c r="AA21" s="25">
         <f t="shared" si="7"/>
-        <v>-2471.3499309597069</v>
+        <v>-2467.8659321480927</v>
       </c>
       <c r="AC21" s="21">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>4.75</v>
       </c>
       <c r="AD21" s="22">
@@ -21231,12 +21231,12 @@
         <v>-2325</v>
       </c>
       <c r="AH21" s="23">
-        <f>IF(AC21&gt;Maturity,"-",EXP(-DomesticHazardRate*AC20)-EXP(-DomesticHazardRate*AC21))</f>
+        <f t="shared" si="27"/>
         <v>6.5283573957795049E-3</v>
       </c>
       <c r="AI21" s="23">
-        <f>IF(AC21&gt;Maturity,"-",EXP(-QuantoHazardRate*AC20)-EXP(-QuantoHazardRate*AC21))</f>
-        <v>7.0957436285764564E-3</v>
+        <f t="shared" si="28"/>
+        <v>7.1496346578089343E-3</v>
       </c>
       <c r="AJ21" s="23">
         <f t="shared" si="14"/>
@@ -21248,10 +21248,10 @@
       </c>
       <c r="AL21" s="25">
         <f t="shared" si="16"/>
-        <v>-10.259613355550689</v>
+        <v>-10.337533465436174</v>
       </c>
       <c r="AN21" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>4.75</v>
       </c>
       <c r="AO21" s="22">
@@ -21263,12 +21263,12 @@
         <v>600000</v>
       </c>
       <c r="AQ21" s="23">
-        <f>IF(AN21&gt;Maturity,"-",EXP(-DomesticHazardRate*AN20)-EXP(-DomesticHazardRate*AN21))</f>
+        <f t="shared" si="30"/>
         <v>6.5283573957795049E-3</v>
       </c>
       <c r="AR21" s="23">
-        <f>IF(AN21&gt;Maturity,"-",EXP(-QuantoHazardRate*AN20)-EXP(-QuantoHazardRate*AN21))</f>
-        <v>7.0957436285764564E-3</v>
+        <f t="shared" si="31"/>
+        <v>7.1496346578089343E-3</v>
       </c>
       <c r="AS21" s="23">
         <f t="shared" si="21"/>
@@ -21280,13 +21280,13 @@
       </c>
       <c r="AU21" s="25">
         <f t="shared" si="23"/>
-        <v>2647.6421562711453</v>
+        <v>2667.7505717254635</v>
       </c>
     </row>
     <row r="22" spans="2:47">
       <c r="P22" s="3"/>
       <c r="R22" s="35">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>5</v>
       </c>
       <c r="S22" s="22">
@@ -21311,7 +21311,7 @@
       </c>
       <c r="X22" s="50">
         <f t="shared" si="4"/>
-        <v>0.84757898197418036</v>
+        <v>0.84632126127469776</v>
       </c>
       <c r="Y22" s="23">
         <f t="shared" si="5"/>
@@ -21323,10 +21323,10 @@
       </c>
       <c r="AA22" s="25">
         <f t="shared" si="7"/>
-        <v>-2390.4842717934325</v>
+        <v>-2386.9370371234322</v>
       </c>
       <c r="AC22" s="21">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>5</v>
       </c>
       <c r="AD22" s="22">
@@ -21346,12 +21346,12 @@
         <v>-2325</v>
       </c>
       <c r="AH22" s="23">
-        <f>IF(AC22&gt;Maturity,"-",EXP(-DomesticHazardRate*AC21)-EXP(-DomesticHazardRate*AC22))</f>
+        <f t="shared" si="27"/>
         <v>6.479577867197106E-3</v>
       </c>
       <c r="AI22" s="23">
-        <f>IF(AC22&gt;Maturity,"-",EXP(-QuantoHazardRate*AC21)-EXP(-QuantoHazardRate*AC22))</f>
-        <v>7.0373139266192153E-3</v>
+        <f t="shared" si="28"/>
+        <v>7.0902347222095985E-3</v>
       </c>
       <c r="AJ22" s="23">
         <f t="shared" si="14"/>
@@ -21363,10 +21363,10 @@
       </c>
       <c r="AL22" s="25">
         <f t="shared" si="16"/>
-        <v>-9.9239059810526182</v>
+        <v>-9.9985340288216591</v>
       </c>
       <c r="AN22" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>5</v>
       </c>
       <c r="AO22" s="22">
@@ -21378,12 +21378,12 @@
         <v>600000</v>
       </c>
       <c r="AQ22" s="23">
-        <f>IF(AN22&gt;Maturity,"-",EXP(-DomesticHazardRate*AN21)-EXP(-DomesticHazardRate*AN22))</f>
+        <f t="shared" si="30"/>
         <v>6.479577867197106E-3</v>
       </c>
       <c r="AR22" s="23">
-        <f>IF(AN22&gt;Maturity,"-",EXP(-QuantoHazardRate*AN21)-EXP(-QuantoHazardRate*AN22))</f>
-        <v>7.0373139266192153E-3</v>
+        <f t="shared" si="31"/>
+        <v>7.0902347222095985E-3</v>
       </c>
       <c r="AS22" s="23">
         <f t="shared" si="21"/>
@@ -21395,7 +21395,7 @@
       </c>
       <c r="AU22" s="25">
         <f t="shared" si="23"/>
-        <v>2561.007995110353</v>
+        <v>2580.2668461475246</v>
       </c>
     </row>
     <row r="23" spans="2:47">
@@ -21413,7 +21413,7 @@
       </c>
       <c r="P23" s="3"/>
       <c r="R23" s="35">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>5.25</v>
       </c>
       <c r="S23" s="22" t="str">
@@ -21453,39 +21453,39 @@
         <v>-</v>
       </c>
       <c r="AC23" s="21">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>5.25</v>
       </c>
       <c r="AD23" s="22" t="str">
-        <f t="shared" ref="AD23:AD44" si="34">IF(AC23&gt;Maturity,"-",-Phi*Notional)</f>
+        <f t="shared" ref="AD23:AD44" si="38">IF(AC23&gt;Maturity,"-",-Phi*Notional)</f>
         <v>-</v>
       </c>
       <c r="AE23" s="24" t="str">
-        <f t="shared" ref="AE23:AE44" si="35">IF(AC23&gt;Maturity,"-",Premium)</f>
+        <f t="shared" ref="AE23:AE44" si="39">IF(AC23&gt;Maturity,"-",Premium)</f>
         <v>-</v>
       </c>
       <c r="AF23" s="41" t="str">
-        <f t="shared" ref="AF23:AF44" si="36">IF(AC23&gt;Maturity,"-",YearFraction/2)</f>
+        <f t="shared" ref="AF23:AF44" si="40">IF(AC23&gt;Maturity,"-",YearFraction/2)</f>
         <v>-</v>
       </c>
       <c r="AG23" s="22" t="str">
-        <f t="shared" ref="AG23:AG44" si="37">IF(AC23&gt;Maturity,"-",AD23*AE23*AF23)</f>
+        <f t="shared" ref="AG23:AG44" si="41">IF(AC23&gt;Maturity,"-",AD23*AE23*AF23)</f>
         <v>-</v>
       </c>
       <c r="AH23" s="23" t="str">
-        <f>IF(AC23&gt;Maturity,"-",EXP(-DomesticHazardRate*AC22)-EXP(-DomesticHazardRate*AC23))</f>
+        <f t="shared" si="27"/>
         <v>-</v>
       </c>
       <c r="AI23" s="23" t="str">
-        <f>IF(AC23&gt;Maturity,"-",EXP(-QuantoHazardRate*AC22)-EXP(-QuantoHazardRate*AC23))</f>
+        <f t="shared" si="28"/>
         <v>-</v>
       </c>
       <c r="AJ23" s="23" t="str">
-        <f t="shared" ref="AJ23:AJ44" si="38">IF(AC23&gt;Maturity,"-",EXP(-ZeroRate*AC23))</f>
+        <f t="shared" ref="AJ23:AJ44" si="42">IF(AC23&gt;Maturity,"-",EXP(-ZeroRate*AC23))</f>
         <v>-</v>
       </c>
       <c r="AK23" s="22" t="str">
-        <f t="shared" ref="AK23:AK44" si="39">IF(AC23&gt;Maturity,"-",AG23*AH23*AJ23)</f>
+        <f t="shared" ref="AK23:AK44" si="43">IF(AC23&gt;Maturity,"-",AG23*AH23*AJ23)</f>
         <v>-</v>
       </c>
       <c r="AL23" s="25" t="str">
@@ -21493,31 +21493,31 @@
         <v>-</v>
       </c>
       <c r="AN23" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>5.25</v>
       </c>
       <c r="AO23" s="22" t="str">
-        <f t="shared" ref="AO23:AO44" si="40">IF(AN23&gt;Maturity,"-",Phi*Notional)</f>
+        <f t="shared" ref="AO23:AO44" si="44">IF(AN23&gt;Maturity,"-",Phi*Notional)</f>
         <v>-</v>
       </c>
       <c r="AP23" s="22" t="str">
-        <f t="shared" ref="AP23:AP44" si="41">IF(AN23&gt;Maturity,"-",Phi*Notional*(1-RecoveryRate))</f>
+        <f t="shared" ref="AP23:AP44" si="45">IF(AN23&gt;Maturity,"-",Phi*Notional*(1-RecoveryRate))</f>
         <v>-</v>
       </c>
       <c r="AQ23" s="23" t="str">
-        <f>IF(AN23&gt;Maturity,"-",EXP(-DomesticHazardRate*AN22)-EXP(-DomesticHazardRate*AN23))</f>
+        <f t="shared" si="30"/>
         <v>-</v>
       </c>
       <c r="AR23" s="23" t="str">
-        <f>IF(AN23&gt;Maturity,"-",EXP(-QuantoHazardRate*AN22)-EXP(-QuantoHazardRate*AN23))</f>
+        <f t="shared" si="31"/>
         <v>-</v>
       </c>
       <c r="AS23" s="23" t="str">
-        <f t="shared" ref="AS23:AS44" si="42">IF(AN23&gt;Maturity,"-",EXP(-ZeroRate*AN23))</f>
+        <f t="shared" ref="AS23:AS44" si="46">IF(AN23&gt;Maturity,"-",EXP(-ZeroRate*AN23))</f>
         <v>-</v>
       </c>
       <c r="AT23" s="22" t="str">
-        <f t="shared" ref="AT23:AT44" si="43">IF(AN23&gt;Maturity,"-",AP23*AQ23*AS23)</f>
+        <f t="shared" ref="AT23:AT44" si="47">IF(AN23&gt;Maturity,"-",AP23*AQ23*AS23)</f>
         <v>-</v>
       </c>
       <c r="AU23" s="25" t="str">
@@ -21535,15 +21535,15 @@
       </c>
       <c r="D24" s="61">
         <f>SUM(D25:D27)</f>
-        <v>4487.4155105993123</v>
+        <v>5126.6017934921692</v>
       </c>
       <c r="E24" s="61">
         <f>D24-C24</f>
-        <v>6666.1812065362392</v>
+        <v>7305.3674894290962</v>
       </c>
       <c r="P24" s="3"/>
       <c r="R24" s="35">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>5.5</v>
       </c>
       <c r="S24" s="22" t="str">
@@ -21583,39 +21583,39 @@
         <v>-</v>
       </c>
       <c r="AC24" s="21">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>5.5</v>
       </c>
       <c r="AD24" s="22" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>-</v>
       </c>
       <c r="AE24" s="24" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>-</v>
       </c>
       <c r="AF24" s="41" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>-</v>
       </c>
       <c r="AG24" s="22" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>-</v>
       </c>
       <c r="AH24" s="23" t="str">
-        <f>IF(AC24&gt;Maturity,"-",EXP(-DomesticHazardRate*AC23)-EXP(-DomesticHazardRate*AC24))</f>
+        <f t="shared" si="27"/>
         <v>-</v>
       </c>
       <c r="AI24" s="23" t="str">
-        <f>IF(AC24&gt;Maturity,"-",EXP(-QuantoHazardRate*AC23)-EXP(-QuantoHazardRate*AC24))</f>
+        <f t="shared" si="28"/>
         <v>-</v>
       </c>
       <c r="AJ24" s="23" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>-</v>
       </c>
       <c r="AK24" s="22" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>-</v>
       </c>
       <c r="AL24" s="25" t="str">
@@ -21623,31 +21623,31 @@
         <v>-</v>
       </c>
       <c r="AN24" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>5.5</v>
       </c>
       <c r="AO24" s="22" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>-</v>
       </c>
       <c r="AP24" s="22" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>-</v>
       </c>
       <c r="AQ24" s="23" t="str">
-        <f>IF(AN24&gt;Maturity,"-",EXP(-DomesticHazardRate*AN23)-EXP(-DomesticHazardRate*AN24))</f>
+        <f t="shared" si="30"/>
         <v>-</v>
       </c>
       <c r="AR24" s="23" t="str">
-        <f>IF(AN24&gt;Maturity,"-",EXP(-QuantoHazardRate*AN23)-EXP(-QuantoHazardRate*AN24))</f>
+        <f t="shared" si="31"/>
         <v>-</v>
       </c>
       <c r="AS24" s="23" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>-</v>
       </c>
       <c r="AT24" s="22" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>-</v>
       </c>
       <c r="AU24" s="25" t="str">
@@ -21665,16 +21665,16 @@
       </c>
       <c r="D25" s="14">
         <f>QuantoPremiumLegTotalPV</f>
-        <v>-66793.950186463466</v>
+        <v>-66747.344094916145</v>
       </c>
       <c r="E25" s="14">
         <f>D25-C25</f>
-        <v>485.04500719846692</v>
+        <v>531.65109874578775</v>
       </c>
       <c r="I25" s="47"/>
       <c r="P25" s="3"/>
       <c r="R25" s="35">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>5.75</v>
       </c>
       <c r="S25" s="22" t="str">
@@ -21714,39 +21714,39 @@
         <v>-</v>
       </c>
       <c r="AC25" s="21">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>5.75</v>
       </c>
       <c r="AD25" s="22" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>-</v>
       </c>
       <c r="AE25" s="24" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>-</v>
       </c>
       <c r="AF25" s="41" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>-</v>
       </c>
       <c r="AG25" s="22" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>-</v>
       </c>
       <c r="AH25" s="23" t="str">
-        <f>IF(AC25&gt;Maturity,"-",EXP(-DomesticHazardRate*AC24)-EXP(-DomesticHazardRate*AC25))</f>
+        <f t="shared" si="27"/>
         <v>-</v>
       </c>
       <c r="AI25" s="23" t="str">
-        <f>IF(AC25&gt;Maturity,"-",EXP(-QuantoHazardRate*AC24)-EXP(-QuantoHazardRate*AC25))</f>
+        <f t="shared" si="28"/>
         <v>-</v>
       </c>
       <c r="AJ25" s="23" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>-</v>
       </c>
       <c r="AK25" s="22" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>-</v>
       </c>
       <c r="AL25" s="25" t="str">
@@ -21754,31 +21754,31 @@
         <v>-</v>
       </c>
       <c r="AN25" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>5.75</v>
       </c>
       <c r="AO25" s="22" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>-</v>
       </c>
       <c r="AP25" s="22" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>-</v>
       </c>
       <c r="AQ25" s="23" t="str">
-        <f>IF(AN25&gt;Maturity,"-",EXP(-DomesticHazardRate*AN24)-EXP(-DomesticHazardRate*AN25))</f>
+        <f t="shared" si="30"/>
         <v>-</v>
       </c>
       <c r="AR25" s="23" t="str">
-        <f>IF(AN25&gt;Maturity,"-",EXP(-QuantoHazardRate*AN24)-EXP(-QuantoHazardRate*AN25))</f>
+        <f t="shared" si="31"/>
         <v>-</v>
       </c>
       <c r="AS25" s="23" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>-</v>
       </c>
       <c r="AT25" s="22" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>-</v>
       </c>
       <c r="AU25" s="25" t="str">
@@ -21796,16 +21796,16 @@
       </c>
       <c r="D26" s="14">
         <f>QuantoAccruedInterestTotalPV</f>
-        <v>-277.28979001241635</v>
+        <v>-279.5949708295467</v>
       </c>
       <c r="E26" s="14">
         <f>D26-C26</f>
-        <v>-24.045077447543036</v>
+        <v>-26.350258264673386</v>
       </c>
       <c r="I26" s="44"/>
       <c r="P26" s="3"/>
       <c r="R26" s="35">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>6</v>
       </c>
       <c r="S26" s="22" t="str">
@@ -21845,39 +21845,39 @@
         <v>-</v>
       </c>
       <c r="AC26" s="21">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>6</v>
       </c>
       <c r="AD26" s="22" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>-</v>
       </c>
       <c r="AE26" s="24" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>-</v>
       </c>
       <c r="AF26" s="41" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>-</v>
       </c>
       <c r="AG26" s="22" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>-</v>
       </c>
       <c r="AH26" s="23" t="str">
-        <f>IF(AC26&gt;Maturity,"-",EXP(-DomesticHazardRate*AC25)-EXP(-DomesticHazardRate*AC26))</f>
+        <f t="shared" si="27"/>
         <v>-</v>
       </c>
       <c r="AI26" s="23" t="str">
-        <f>IF(AC26&gt;Maturity,"-",EXP(-QuantoHazardRate*AC25)-EXP(-QuantoHazardRate*AC26))</f>
+        <f t="shared" si="28"/>
         <v>-</v>
       </c>
       <c r="AJ26" s="23" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>-</v>
       </c>
       <c r="AK26" s="22" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>-</v>
       </c>
       <c r="AL26" s="25" t="str">
@@ -21885,31 +21885,31 @@
         <v>-</v>
       </c>
       <c r="AN26" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>6</v>
       </c>
       <c r="AO26" s="22" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>-</v>
       </c>
       <c r="AP26" s="22" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>-</v>
       </c>
       <c r="AQ26" s="23" t="str">
-        <f>IF(AN26&gt;Maturity,"-",EXP(-DomesticHazardRate*AN25)-EXP(-DomesticHazardRate*AN26))</f>
+        <f t="shared" si="30"/>
         <v>-</v>
       </c>
       <c r="AR26" s="23" t="str">
-        <f>IF(AN26&gt;Maturity,"-",EXP(-QuantoHazardRate*AN25)-EXP(-QuantoHazardRate*AN26))</f>
+        <f t="shared" si="31"/>
         <v>-</v>
       </c>
       <c r="AS26" s="23" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>-</v>
       </c>
       <c r="AT26" s="22" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>-</v>
       </c>
       <c r="AU26" s="25" t="str">
@@ -21927,16 +21927,16 @@
       </c>
       <c r="D27" s="15">
         <f>QuantoProtectionLegTotalPV</f>
-        <v>71558.655487075201</v>
+        <v>72153.540859237866</v>
       </c>
       <c r="E27" s="15">
         <f>D27-C27</f>
-        <v>6205.1812767853189</v>
+        <v>6800.0666489479845</v>
       </c>
       <c r="I27" s="63"/>
       <c r="P27" s="3"/>
       <c r="R27" s="35">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>6.25</v>
       </c>
       <c r="S27" s="22" t="str">
@@ -21976,39 +21976,39 @@
         <v>-</v>
       </c>
       <c r="AC27" s="21">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>6.25</v>
       </c>
       <c r="AD27" s="22" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>-</v>
       </c>
       <c r="AE27" s="24" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>-</v>
       </c>
       <c r="AF27" s="41" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>-</v>
       </c>
       <c r="AG27" s="22" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>-</v>
       </c>
       <c r="AH27" s="23" t="str">
-        <f>IF(AC27&gt;Maturity,"-",EXP(-DomesticHazardRate*AC26)-EXP(-DomesticHazardRate*AC27))</f>
+        <f t="shared" si="27"/>
         <v>-</v>
       </c>
       <c r="AI27" s="23" t="str">
-        <f>IF(AC27&gt;Maturity,"-",EXP(-QuantoHazardRate*AC26)-EXP(-QuantoHazardRate*AC27))</f>
+        <f t="shared" si="28"/>
         <v>-</v>
       </c>
       <c r="AJ27" s="23" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>-</v>
       </c>
       <c r="AK27" s="22" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>-</v>
       </c>
       <c r="AL27" s="25" t="str">
@@ -22016,31 +22016,31 @@
         <v>-</v>
       </c>
       <c r="AN27" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>6.25</v>
       </c>
       <c r="AO27" s="22" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>-</v>
       </c>
       <c r="AP27" s="22" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>-</v>
       </c>
       <c r="AQ27" s="23" t="str">
-        <f>IF(AN27&gt;Maturity,"-",EXP(-DomesticHazardRate*AN26)-EXP(-DomesticHazardRate*AN27))</f>
+        <f t="shared" si="30"/>
         <v>-</v>
       </c>
       <c r="AR27" s="23" t="str">
-        <f>IF(AN27&gt;Maturity,"-",EXP(-QuantoHazardRate*AN26)-EXP(-QuantoHazardRate*AN27))</f>
+        <f t="shared" si="31"/>
         <v>-</v>
       </c>
       <c r="AS27" s="23" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>-</v>
       </c>
       <c r="AT27" s="22" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>-</v>
       </c>
       <c r="AU27" s="25" t="str">
@@ -22051,7 +22051,7 @@
     <row r="28" spans="2:47">
       <c r="P28" s="3"/>
       <c r="R28" s="35">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>6.5</v>
       </c>
       <c r="S28" s="22" t="str">
@@ -22091,39 +22091,39 @@
         <v>-</v>
       </c>
       <c r="AC28" s="21">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>6.5</v>
       </c>
       <c r="AD28" s="22" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>-</v>
       </c>
       <c r="AE28" s="24" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>-</v>
       </c>
       <c r="AF28" s="41" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>-</v>
       </c>
       <c r="AG28" s="22" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>-</v>
       </c>
       <c r="AH28" s="23" t="str">
-        <f>IF(AC28&gt;Maturity,"-",EXP(-DomesticHazardRate*AC27)-EXP(-DomesticHazardRate*AC28))</f>
+        <f t="shared" si="27"/>
         <v>-</v>
       </c>
       <c r="AI28" s="23" t="str">
-        <f>IF(AC28&gt;Maturity,"-",EXP(-QuantoHazardRate*AC27)-EXP(-QuantoHazardRate*AC28))</f>
+        <f t="shared" si="28"/>
         <v>-</v>
       </c>
       <c r="AJ28" s="23" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>-</v>
       </c>
       <c r="AK28" s="22" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>-</v>
       </c>
       <c r="AL28" s="25" t="str">
@@ -22131,31 +22131,31 @@
         <v>-</v>
       </c>
       <c r="AN28" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>6.5</v>
       </c>
       <c r="AO28" s="22" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>-</v>
       </c>
       <c r="AP28" s="22" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>-</v>
       </c>
       <c r="AQ28" s="23" t="str">
-        <f>IF(AN28&gt;Maturity,"-",EXP(-DomesticHazardRate*AN27)-EXP(-DomesticHazardRate*AN28))</f>
+        <f t="shared" si="30"/>
         <v>-</v>
       </c>
       <c r="AR28" s="23" t="str">
-        <f>IF(AN28&gt;Maturity,"-",EXP(-QuantoHazardRate*AN27)-EXP(-QuantoHazardRate*AN28))</f>
+        <f t="shared" si="31"/>
         <v>-</v>
       </c>
       <c r="AS28" s="23" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>-</v>
       </c>
       <c r="AT28" s="22" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>-</v>
       </c>
       <c r="AU28" s="25" t="str">
@@ -22178,7 +22178,7 @@
       </c>
       <c r="P29" s="3"/>
       <c r="R29" s="35">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>6.75</v>
       </c>
       <c r="S29" s="22" t="str">
@@ -22218,39 +22218,39 @@
         <v>-</v>
       </c>
       <c r="AC29" s="21">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>6.75</v>
       </c>
       <c r="AD29" s="22" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>-</v>
       </c>
       <c r="AE29" s="24" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>-</v>
       </c>
       <c r="AF29" s="41" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>-</v>
       </c>
       <c r="AG29" s="22" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>-</v>
       </c>
       <c r="AH29" s="23" t="str">
-        <f>IF(AC29&gt;Maturity,"-",EXP(-DomesticHazardRate*AC28)-EXP(-DomesticHazardRate*AC29))</f>
+        <f t="shared" si="27"/>
         <v>-</v>
       </c>
       <c r="AI29" s="23" t="str">
-        <f>IF(AC29&gt;Maturity,"-",EXP(-QuantoHazardRate*AC28)-EXP(-QuantoHazardRate*AC29))</f>
+        <f t="shared" si="28"/>
         <v>-</v>
       </c>
       <c r="AJ29" s="23" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>-</v>
       </c>
       <c r="AK29" s="22" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>-</v>
       </c>
       <c r="AL29" s="25" t="str">
@@ -22258,31 +22258,31 @@
         <v>-</v>
       </c>
       <c r="AN29" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>6.75</v>
       </c>
       <c r="AO29" s="22" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>-</v>
       </c>
       <c r="AP29" s="22" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>-</v>
       </c>
       <c r="AQ29" s="23" t="str">
-        <f>IF(AN29&gt;Maturity,"-",EXP(-DomesticHazardRate*AN28)-EXP(-DomesticHazardRate*AN29))</f>
+        <f t="shared" si="30"/>
         <v>-</v>
       </c>
       <c r="AR29" s="23" t="str">
-        <f>IF(AN29&gt;Maturity,"-",EXP(-QuantoHazardRate*AN28)-EXP(-QuantoHazardRate*AN29))</f>
+        <f t="shared" si="31"/>
         <v>-</v>
       </c>
       <c r="AS29" s="23" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>-</v>
       </c>
       <c r="AT29" s="22" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>-</v>
       </c>
       <c r="AU29" s="25" t="str">
@@ -22300,15 +22300,15 @@
       </c>
       <c r="D30" s="62">
         <f>D31/D32</f>
-        <v>1.984960311920678E-2</v>
+        <v>2.0028593072158162E-2</v>
       </c>
       <c r="E30" s="62">
         <f>D30-C30</f>
-        <v>1.8519462699594924E-3</v>
+        <v>2.0309362229108743E-3</v>
       </c>
       <c r="P30" s="3"/>
       <c r="R30" s="35">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>7</v>
       </c>
       <c r="S30" s="22" t="str">
@@ -22348,39 +22348,39 @@
         <v>-</v>
       </c>
       <c r="AC30" s="21">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>7</v>
       </c>
       <c r="AD30" s="22" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>-</v>
       </c>
       <c r="AE30" s="24" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>-</v>
       </c>
       <c r="AF30" s="41" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>-</v>
       </c>
       <c r="AG30" s="22" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>-</v>
       </c>
       <c r="AH30" s="23" t="str">
-        <f>IF(AC30&gt;Maturity,"-",EXP(-DomesticHazardRate*AC29)-EXP(-DomesticHazardRate*AC30))</f>
+        <f t="shared" si="27"/>
         <v>-</v>
       </c>
       <c r="AI30" s="23" t="str">
-        <f>IF(AC30&gt;Maturity,"-",EXP(-QuantoHazardRate*AC29)-EXP(-QuantoHazardRate*AC30))</f>
+        <f t="shared" si="28"/>
         <v>-</v>
       </c>
       <c r="AJ30" s="23" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>-</v>
       </c>
       <c r="AK30" s="22" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>-</v>
       </c>
       <c r="AL30" s="25" t="str">
@@ -22388,31 +22388,31 @@
         <v>-</v>
       </c>
       <c r="AN30" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>7</v>
       </c>
       <c r="AO30" s="22" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>-</v>
       </c>
       <c r="AP30" s="22" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>-</v>
       </c>
       <c r="AQ30" s="23" t="str">
-        <f>IF(AN30&gt;Maturity,"-",EXP(-DomesticHazardRate*AN29)-EXP(-DomesticHazardRate*AN30))</f>
+        <f t="shared" si="30"/>
         <v>-</v>
       </c>
       <c r="AR30" s="23" t="str">
-        <f>IF(AN30&gt;Maturity,"-",EXP(-QuantoHazardRate*AN29)-EXP(-QuantoHazardRate*AN30))</f>
+        <f t="shared" si="31"/>
         <v>-</v>
       </c>
       <c r="AS30" s="23" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>-</v>
       </c>
       <c r="AT30" s="22" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>-</v>
       </c>
       <c r="AU30" s="25" t="str">
@@ -22430,15 +22430,15 @@
       </c>
       <c r="D31" s="14">
         <f>-QuantoProtectionLegTotalPV-QuantoAccruedInterestTotalPV</f>
-        <v>-71281.365697062778</v>
+        <v>-71873.945888408314</v>
       </c>
       <c r="E31" s="14">
         <f>D31-C31</f>
-        <v>-6181.1361993377723</v>
+        <v>-6773.7163906833084</v>
       </c>
       <c r="P31" s="3"/>
       <c r="R31" s="35">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>7.25</v>
       </c>
       <c r="S31" s="22" t="str">
@@ -22478,39 +22478,39 @@
         <v>-</v>
       </c>
       <c r="AC31" s="21">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>7.25</v>
       </c>
       <c r="AD31" s="22" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>-</v>
       </c>
       <c r="AE31" s="24" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>-</v>
       </c>
       <c r="AF31" s="41" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>-</v>
       </c>
       <c r="AG31" s="22" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>-</v>
       </c>
       <c r="AH31" s="23" t="str">
-        <f>IF(AC31&gt;Maturity,"-",EXP(-DomesticHazardRate*AC30)-EXP(-DomesticHazardRate*AC31))</f>
+        <f t="shared" si="27"/>
         <v>-</v>
       </c>
       <c r="AI31" s="23" t="str">
-        <f>IF(AC31&gt;Maturity,"-",EXP(-QuantoHazardRate*AC30)-EXP(-QuantoHazardRate*AC31))</f>
+        <f t="shared" si="28"/>
         <v>-</v>
       </c>
       <c r="AJ31" s="23" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>-</v>
       </c>
       <c r="AK31" s="22" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>-</v>
       </c>
       <c r="AL31" s="25" t="str">
@@ -22518,31 +22518,31 @@
         <v>-</v>
       </c>
       <c r="AN31" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>7.25</v>
       </c>
       <c r="AO31" s="22" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>-</v>
       </c>
       <c r="AP31" s="22" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>-</v>
       </c>
       <c r="AQ31" s="23" t="str">
-        <f>IF(AN31&gt;Maturity,"-",EXP(-DomesticHazardRate*AN30)-EXP(-DomesticHazardRate*AN31))</f>
+        <f t="shared" si="30"/>
         <v>-</v>
       </c>
       <c r="AR31" s="23" t="str">
-        <f>IF(AN31&gt;Maturity,"-",EXP(-QuantoHazardRate*AN30)-EXP(-QuantoHazardRate*AN31))</f>
+        <f t="shared" si="31"/>
         <v>-</v>
       </c>
       <c r="AS31" s="23" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>-</v>
       </c>
       <c r="AT31" s="22" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>-</v>
       </c>
       <c r="AU31" s="25" t="str">
@@ -22560,15 +22560,15 @@
       </c>
       <c r="D32" s="52">
         <f>SUMPRODUCT(S3:S44,U3:U44,X3:X44,Y3:Y44)</f>
-        <v>-3591072.590670079</v>
+        <v>-3588566.8868234493</v>
       </c>
       <c r="E32" s="15">
         <f>D32-C32</f>
-        <v>26077.688559057657</v>
+        <v>28583.392405687366</v>
       </c>
       <c r="P32" s="3"/>
       <c r="R32" s="35">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>7.5</v>
       </c>
       <c r="S32" s="22" t="str">
@@ -22608,39 +22608,39 @@
         <v>-</v>
       </c>
       <c r="AC32" s="21">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>7.5</v>
       </c>
       <c r="AD32" s="22" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>-</v>
       </c>
       <c r="AE32" s="24" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>-</v>
       </c>
       <c r="AF32" s="41" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>-</v>
       </c>
       <c r="AG32" s="22" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>-</v>
       </c>
       <c r="AH32" s="23" t="str">
-        <f>IF(AC32&gt;Maturity,"-",EXP(-DomesticHazardRate*AC31)-EXP(-DomesticHazardRate*AC32))</f>
+        <f t="shared" si="27"/>
         <v>-</v>
       </c>
       <c r="AI32" s="23" t="str">
-        <f>IF(AC32&gt;Maturity,"-",EXP(-QuantoHazardRate*AC31)-EXP(-QuantoHazardRate*AC32))</f>
+        <f t="shared" si="28"/>
         <v>-</v>
       </c>
       <c r="AJ32" s="23" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>-</v>
       </c>
       <c r="AK32" s="22" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>-</v>
       </c>
       <c r="AL32" s="25" t="str">
@@ -22648,31 +22648,31 @@
         <v>-</v>
       </c>
       <c r="AN32" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>7.5</v>
       </c>
       <c r="AO32" s="22" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>-</v>
       </c>
       <c r="AP32" s="22" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>-</v>
       </c>
       <c r="AQ32" s="23" t="str">
-        <f>IF(AN32&gt;Maturity,"-",EXP(-DomesticHazardRate*AN31)-EXP(-DomesticHazardRate*AN32))</f>
+        <f t="shared" si="30"/>
         <v>-</v>
       </c>
       <c r="AR32" s="23" t="str">
-        <f>IF(AN32&gt;Maturity,"-",EXP(-QuantoHazardRate*AN31)-EXP(-QuantoHazardRate*AN32))</f>
+        <f t="shared" si="31"/>
         <v>-</v>
       </c>
       <c r="AS32" s="23" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>-</v>
       </c>
       <c r="AT32" s="22" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>-</v>
       </c>
       <c r="AU32" s="25" t="str">
@@ -22683,7 +22683,7 @@
     <row r="33" spans="8:47">
       <c r="P33" s="3"/>
       <c r="R33" s="35">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>7.75</v>
       </c>
       <c r="S33" s="22" t="str">
@@ -22723,39 +22723,39 @@
         <v>-</v>
       </c>
       <c r="AC33" s="21">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>7.75</v>
       </c>
       <c r="AD33" s="22" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>-</v>
       </c>
       <c r="AE33" s="24" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>-</v>
       </c>
       <c r="AF33" s="41" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>-</v>
       </c>
       <c r="AG33" s="22" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>-</v>
       </c>
       <c r="AH33" s="23" t="str">
-        <f>IF(AC33&gt;Maturity,"-",EXP(-DomesticHazardRate*AC32)-EXP(-DomesticHazardRate*AC33))</f>
+        <f t="shared" si="27"/>
         <v>-</v>
       </c>
       <c r="AI33" s="23" t="str">
-        <f>IF(AC33&gt;Maturity,"-",EXP(-QuantoHazardRate*AC32)-EXP(-QuantoHazardRate*AC33))</f>
+        <f t="shared" si="28"/>
         <v>-</v>
       </c>
       <c r="AJ33" s="23" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>-</v>
       </c>
       <c r="AK33" s="22" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>-</v>
       </c>
       <c r="AL33" s="25" t="str">
@@ -22763,31 +22763,31 @@
         <v>-</v>
       </c>
       <c r="AN33" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>7.75</v>
       </c>
       <c r="AO33" s="22" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>-</v>
       </c>
       <c r="AP33" s="22" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>-</v>
       </c>
       <c r="AQ33" s="23" t="str">
-        <f>IF(AN33&gt;Maturity,"-",EXP(-DomesticHazardRate*AN32)-EXP(-DomesticHazardRate*AN33))</f>
+        <f t="shared" si="30"/>
         <v>-</v>
       </c>
       <c r="AR33" s="23" t="str">
-        <f>IF(AN33&gt;Maturity,"-",EXP(-QuantoHazardRate*AN32)-EXP(-QuantoHazardRate*AN33))</f>
+        <f t="shared" si="31"/>
         <v>-</v>
       </c>
       <c r="AS33" s="23" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>-</v>
       </c>
       <c r="AT33" s="22" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>-</v>
       </c>
       <c r="AU33" s="25" t="str">
@@ -22798,7 +22798,7 @@
     <row r="34" spans="8:47">
       <c r="P34" s="3"/>
       <c r="R34" s="35">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>8</v>
       </c>
       <c r="S34" s="22" t="str">
@@ -22838,39 +22838,39 @@
         <v>-</v>
       </c>
       <c r="AC34" s="21">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>8</v>
       </c>
       <c r="AD34" s="22" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>-</v>
       </c>
       <c r="AE34" s="24" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>-</v>
       </c>
       <c r="AF34" s="41" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>-</v>
       </c>
       <c r="AG34" s="22" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>-</v>
       </c>
       <c r="AH34" s="23" t="str">
-        <f>IF(AC34&gt;Maturity,"-",EXP(-DomesticHazardRate*AC33)-EXP(-DomesticHazardRate*AC34))</f>
+        <f t="shared" si="27"/>
         <v>-</v>
       </c>
       <c r="AI34" s="23" t="str">
-        <f>IF(AC34&gt;Maturity,"-",EXP(-QuantoHazardRate*AC33)-EXP(-QuantoHazardRate*AC34))</f>
+        <f t="shared" si="28"/>
         <v>-</v>
       </c>
       <c r="AJ34" s="23" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>-</v>
       </c>
       <c r="AK34" s="22" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>-</v>
       </c>
       <c r="AL34" s="25" t="str">
@@ -22878,31 +22878,31 @@
         <v>-</v>
       </c>
       <c r="AN34" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>8</v>
       </c>
       <c r="AO34" s="22" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>-</v>
       </c>
       <c r="AP34" s="22" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>-</v>
       </c>
       <c r="AQ34" s="23" t="str">
-        <f>IF(AN34&gt;Maturity,"-",EXP(-DomesticHazardRate*AN33)-EXP(-DomesticHazardRate*AN34))</f>
+        <f t="shared" si="30"/>
         <v>-</v>
       </c>
       <c r="AR34" s="23" t="str">
-        <f>IF(AN34&gt;Maturity,"-",EXP(-QuantoHazardRate*AN33)-EXP(-QuantoHazardRate*AN34))</f>
+        <f t="shared" si="31"/>
         <v>-</v>
       </c>
       <c r="AS34" s="23" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>-</v>
       </c>
       <c r="AT34" s="22" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>-</v>
       </c>
       <c r="AU34" s="25" t="str">
@@ -22913,7 +22913,7 @@
     <row r="35" spans="8:47">
       <c r="P35" s="3"/>
       <c r="R35" s="35">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>8.25</v>
       </c>
       <c r="S35" s="22" t="str">
@@ -22953,39 +22953,39 @@
         <v>-</v>
       </c>
       <c r="AC35" s="21">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>8.25</v>
       </c>
       <c r="AD35" s="22" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>-</v>
       </c>
       <c r="AE35" s="24" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>-</v>
       </c>
       <c r="AF35" s="41" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>-</v>
       </c>
       <c r="AG35" s="22" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>-</v>
       </c>
       <c r="AH35" s="23" t="str">
-        <f>IF(AC35&gt;Maturity,"-",EXP(-DomesticHazardRate*AC34)-EXP(-DomesticHazardRate*AC35))</f>
+        <f t="shared" si="27"/>
         <v>-</v>
       </c>
       <c r="AI35" s="23" t="str">
-        <f>IF(AC35&gt;Maturity,"-",EXP(-QuantoHazardRate*AC34)-EXP(-QuantoHazardRate*AC35))</f>
+        <f t="shared" si="28"/>
         <v>-</v>
       </c>
       <c r="AJ35" s="23" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>-</v>
       </c>
       <c r="AK35" s="22" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>-</v>
       </c>
       <c r="AL35" s="25" t="str">
@@ -22993,31 +22993,31 @@
         <v>-</v>
       </c>
       <c r="AN35" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>8.25</v>
       </c>
       <c r="AO35" s="22" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>-</v>
       </c>
       <c r="AP35" s="22" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>-</v>
       </c>
       <c r="AQ35" s="23" t="str">
-        <f>IF(AN35&gt;Maturity,"-",EXP(-DomesticHazardRate*AN34)-EXP(-DomesticHazardRate*AN35))</f>
+        <f t="shared" si="30"/>
         <v>-</v>
       </c>
       <c r="AR35" s="23" t="str">
-        <f>IF(AN35&gt;Maturity,"-",EXP(-QuantoHazardRate*AN34)-EXP(-QuantoHazardRate*AN35))</f>
+        <f t="shared" si="31"/>
         <v>-</v>
       </c>
       <c r="AS35" s="23" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>-</v>
       </c>
       <c r="AT35" s="22" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>-</v>
       </c>
       <c r="AU35" s="25" t="str">
@@ -23036,7 +23036,7 @@
       <c r="O36" s="44"/>
       <c r="P36" s="3"/>
       <c r="R36" s="35">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>8.5</v>
       </c>
       <c r="S36" s="22" t="str">
@@ -23076,39 +23076,39 @@
         <v>-</v>
       </c>
       <c r="AC36" s="21">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>8.5</v>
       </c>
       <c r="AD36" s="22" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>-</v>
       </c>
       <c r="AE36" s="24" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>-</v>
       </c>
       <c r="AF36" s="41" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>-</v>
       </c>
       <c r="AG36" s="22" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>-</v>
       </c>
       <c r="AH36" s="23" t="str">
-        <f>IF(AC36&gt;Maturity,"-",EXP(-DomesticHazardRate*AC35)-EXP(-DomesticHazardRate*AC36))</f>
+        <f t="shared" si="27"/>
         <v>-</v>
       </c>
       <c r="AI36" s="23" t="str">
-        <f>IF(AC36&gt;Maturity,"-",EXP(-QuantoHazardRate*AC35)-EXP(-QuantoHazardRate*AC36))</f>
+        <f t="shared" si="28"/>
         <v>-</v>
       </c>
       <c r="AJ36" s="23" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>-</v>
       </c>
       <c r="AK36" s="22" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>-</v>
       </c>
       <c r="AL36" s="25" t="str">
@@ -23116,31 +23116,31 @@
         <v>-</v>
       </c>
       <c r="AN36" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>8.5</v>
       </c>
       <c r="AO36" s="22" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>-</v>
       </c>
       <c r="AP36" s="22" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>-</v>
       </c>
       <c r="AQ36" s="23" t="str">
-        <f>IF(AN36&gt;Maturity,"-",EXP(-DomesticHazardRate*AN35)-EXP(-DomesticHazardRate*AN36))</f>
+        <f t="shared" si="30"/>
         <v>-</v>
       </c>
       <c r="AR36" s="23" t="str">
-        <f>IF(AN36&gt;Maturity,"-",EXP(-QuantoHazardRate*AN35)-EXP(-QuantoHazardRate*AN36))</f>
+        <f t="shared" si="31"/>
         <v>-</v>
       </c>
       <c r="AS36" s="23" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>-</v>
       </c>
       <c r="AT36" s="22" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>-</v>
       </c>
       <c r="AU36" s="25" t="str">
@@ -23151,7 +23151,7 @@
     <row r="37" spans="8:47">
       <c r="P37" s="3"/>
       <c r="R37" s="35">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>8.75</v>
       </c>
       <c r="S37" s="22" t="str">
@@ -23191,39 +23191,39 @@
         <v>-</v>
       </c>
       <c r="AC37" s="21">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>8.75</v>
       </c>
       <c r="AD37" s="22" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>-</v>
       </c>
       <c r="AE37" s="24" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>-</v>
       </c>
       <c r="AF37" s="41" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>-</v>
       </c>
       <c r="AG37" s="22" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>-</v>
       </c>
       <c r="AH37" s="23" t="str">
-        <f>IF(AC37&gt;Maturity,"-",EXP(-DomesticHazardRate*AC36)-EXP(-DomesticHazardRate*AC37))</f>
+        <f t="shared" si="27"/>
         <v>-</v>
       </c>
       <c r="AI37" s="23" t="str">
-        <f>IF(AC37&gt;Maturity,"-",EXP(-QuantoHazardRate*AC36)-EXP(-QuantoHazardRate*AC37))</f>
+        <f t="shared" si="28"/>
         <v>-</v>
       </c>
       <c r="AJ37" s="23" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>-</v>
       </c>
       <c r="AK37" s="22" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>-</v>
       </c>
       <c r="AL37" s="25" t="str">
@@ -23231,31 +23231,31 @@
         <v>-</v>
       </c>
       <c r="AN37" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>8.75</v>
       </c>
       <c r="AO37" s="22" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>-</v>
       </c>
       <c r="AP37" s="22" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>-</v>
       </c>
       <c r="AQ37" s="23" t="str">
-        <f>IF(AN37&gt;Maturity,"-",EXP(-DomesticHazardRate*AN36)-EXP(-DomesticHazardRate*AN37))</f>
+        <f t="shared" si="30"/>
         <v>-</v>
       </c>
       <c r="AR37" s="23" t="str">
-        <f>IF(AN37&gt;Maturity,"-",EXP(-QuantoHazardRate*AN36)-EXP(-QuantoHazardRate*AN37))</f>
+        <f t="shared" si="31"/>
         <v>-</v>
       </c>
       <c r="AS37" s="23" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>-</v>
       </c>
       <c r="AT37" s="22" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>-</v>
       </c>
       <c r="AU37" s="25" t="str">
@@ -23266,7 +23266,7 @@
     <row r="38" spans="8:47">
       <c r="P38" s="3"/>
       <c r="R38" s="35">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>9</v>
       </c>
       <c r="S38" s="22" t="str">
@@ -23306,39 +23306,39 @@
         <v>-</v>
       </c>
       <c r="AC38" s="21">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>9</v>
       </c>
       <c r="AD38" s="22" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>-</v>
       </c>
       <c r="AE38" s="24" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>-</v>
       </c>
       <c r="AF38" s="41" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>-</v>
       </c>
       <c r="AG38" s="22" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>-</v>
       </c>
       <c r="AH38" s="23" t="str">
-        <f>IF(AC38&gt;Maturity,"-",EXP(-DomesticHazardRate*AC37)-EXP(-DomesticHazardRate*AC38))</f>
+        <f t="shared" si="27"/>
         <v>-</v>
       </c>
       <c r="AI38" s="23" t="str">
-        <f>IF(AC38&gt;Maturity,"-",EXP(-QuantoHazardRate*AC37)-EXP(-QuantoHazardRate*AC38))</f>
+        <f t="shared" si="28"/>
         <v>-</v>
       </c>
       <c r="AJ38" s="23" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>-</v>
       </c>
       <c r="AK38" s="22" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>-</v>
       </c>
       <c r="AL38" s="25" t="str">
@@ -23346,31 +23346,31 @@
         <v>-</v>
       </c>
       <c r="AN38" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>9</v>
       </c>
       <c r="AO38" s="22" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>-</v>
       </c>
       <c r="AP38" s="22" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>-</v>
       </c>
       <c r="AQ38" s="23" t="str">
-        <f>IF(AN38&gt;Maturity,"-",EXP(-DomesticHazardRate*AN37)-EXP(-DomesticHazardRate*AN38))</f>
+        <f t="shared" si="30"/>
         <v>-</v>
       </c>
       <c r="AR38" s="23" t="str">
-        <f>IF(AN38&gt;Maturity,"-",EXP(-QuantoHazardRate*AN37)-EXP(-QuantoHazardRate*AN38))</f>
+        <f t="shared" si="31"/>
         <v>-</v>
       </c>
       <c r="AS38" s="23" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>-</v>
       </c>
       <c r="AT38" s="22" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>-</v>
       </c>
       <c r="AU38" s="25" t="str">
@@ -23381,7 +23381,7 @@
     <row r="39" spans="8:47">
       <c r="P39" s="3"/>
       <c r="R39" s="35">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>9.25</v>
       </c>
       <c r="S39" s="22" t="str">
@@ -23421,39 +23421,39 @@
         <v>-</v>
       </c>
       <c r="AC39" s="21">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>9.25</v>
       </c>
       <c r="AD39" s="22" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>-</v>
       </c>
       <c r="AE39" s="24" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>-</v>
       </c>
       <c r="AF39" s="41" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>-</v>
       </c>
       <c r="AG39" s="22" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>-</v>
       </c>
       <c r="AH39" s="23" t="str">
-        <f>IF(AC39&gt;Maturity,"-",EXP(-DomesticHazardRate*AC38)-EXP(-DomesticHazardRate*AC39))</f>
+        <f t="shared" si="27"/>
         <v>-</v>
       </c>
       <c r="AI39" s="23" t="str">
-        <f>IF(AC39&gt;Maturity,"-",EXP(-QuantoHazardRate*AC38)-EXP(-QuantoHazardRate*AC39))</f>
+        <f t="shared" si="28"/>
         <v>-</v>
       </c>
       <c r="AJ39" s="23" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>-</v>
       </c>
       <c r="AK39" s="22" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>-</v>
       </c>
       <c r="AL39" s="25" t="str">
@@ -23461,31 +23461,31 @@
         <v>-</v>
       </c>
       <c r="AN39" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>9.25</v>
       </c>
       <c r="AO39" s="22" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>-</v>
       </c>
       <c r="AP39" s="22" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>-</v>
       </c>
       <c r="AQ39" s="23" t="str">
-        <f>IF(AN39&gt;Maturity,"-",EXP(-DomesticHazardRate*AN38)-EXP(-DomesticHazardRate*AN39))</f>
+        <f t="shared" si="30"/>
         <v>-</v>
       </c>
       <c r="AR39" s="23" t="str">
-        <f>IF(AN39&gt;Maturity,"-",EXP(-QuantoHazardRate*AN38)-EXP(-QuantoHazardRate*AN39))</f>
+        <f t="shared" si="31"/>
         <v>-</v>
       </c>
       <c r="AS39" s="23" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>-</v>
       </c>
       <c r="AT39" s="22" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>-</v>
       </c>
       <c r="AU39" s="25" t="str">
@@ -23496,7 +23496,7 @@
     <row r="40" spans="8:47">
       <c r="P40" s="3"/>
       <c r="R40" s="35">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>9.5</v>
       </c>
       <c r="S40" s="22" t="str">
@@ -23536,39 +23536,39 @@
         <v>-</v>
       </c>
       <c r="AC40" s="21">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>9.5</v>
       </c>
       <c r="AD40" s="22" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>-</v>
       </c>
       <c r="AE40" s="24" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>-</v>
       </c>
       <c r="AF40" s="41" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>-</v>
       </c>
       <c r="AG40" s="22" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>-</v>
       </c>
       <c r="AH40" s="23" t="str">
-        <f>IF(AC40&gt;Maturity,"-",EXP(-DomesticHazardRate*AC39)-EXP(-DomesticHazardRate*AC40))</f>
+        <f t="shared" si="27"/>
         <v>-</v>
       </c>
       <c r="AI40" s="23" t="str">
-        <f>IF(AC40&gt;Maturity,"-",EXP(-QuantoHazardRate*AC39)-EXP(-QuantoHazardRate*AC40))</f>
+        <f t="shared" si="28"/>
         <v>-</v>
       </c>
       <c r="AJ40" s="23" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>-</v>
       </c>
       <c r="AK40" s="22" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>-</v>
       </c>
       <c r="AL40" s="25" t="str">
@@ -23576,31 +23576,31 @@
         <v>-</v>
       </c>
       <c r="AN40" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>9.5</v>
       </c>
       <c r="AO40" s="22" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>-</v>
       </c>
       <c r="AP40" s="22" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>-</v>
       </c>
       <c r="AQ40" s="23" t="str">
-        <f>IF(AN40&gt;Maturity,"-",EXP(-DomesticHazardRate*AN39)-EXP(-DomesticHazardRate*AN40))</f>
+        <f t="shared" si="30"/>
         <v>-</v>
       </c>
       <c r="AR40" s="23" t="str">
-        <f>IF(AN40&gt;Maturity,"-",EXP(-QuantoHazardRate*AN39)-EXP(-QuantoHazardRate*AN40))</f>
+        <f t="shared" si="31"/>
         <v>-</v>
       </c>
       <c r="AS40" s="23" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>-</v>
       </c>
       <c r="AT40" s="22" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>-</v>
       </c>
       <c r="AU40" s="25" t="str">
@@ -23611,7 +23611,7 @@
     <row r="41" spans="8:47">
       <c r="P41" s="3"/>
       <c r="R41" s="35">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>9.75</v>
       </c>
       <c r="S41" s="22" t="str">
@@ -23651,39 +23651,39 @@
         <v>-</v>
       </c>
       <c r="AC41" s="21">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>9.75</v>
       </c>
       <c r="AD41" s="22" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>-</v>
       </c>
       <c r="AE41" s="24" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>-</v>
       </c>
       <c r="AF41" s="41" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>-</v>
       </c>
       <c r="AG41" s="22" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>-</v>
       </c>
       <c r="AH41" s="23" t="str">
-        <f>IF(AC41&gt;Maturity,"-",EXP(-DomesticHazardRate*AC40)-EXP(-DomesticHazardRate*AC41))</f>
+        <f t="shared" si="27"/>
         <v>-</v>
       </c>
       <c r="AI41" s="23" t="str">
-        <f>IF(AC41&gt;Maturity,"-",EXP(-QuantoHazardRate*AC40)-EXP(-QuantoHazardRate*AC41))</f>
+        <f t="shared" si="28"/>
         <v>-</v>
       </c>
       <c r="AJ41" s="23" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>-</v>
       </c>
       <c r="AK41" s="22" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>-</v>
       </c>
       <c r="AL41" s="25" t="str">
@@ -23691,31 +23691,31 @@
         <v>-</v>
       </c>
       <c r="AN41" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>9.75</v>
       </c>
       <c r="AO41" s="22" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>-</v>
       </c>
       <c r="AP41" s="22" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>-</v>
       </c>
       <c r="AQ41" s="23" t="str">
-        <f>IF(AN41&gt;Maturity,"-",EXP(-DomesticHazardRate*AN40)-EXP(-DomesticHazardRate*AN41))</f>
+        <f t="shared" si="30"/>
         <v>-</v>
       </c>
       <c r="AR41" s="23" t="str">
-        <f>IF(AN41&gt;Maturity,"-",EXP(-QuantoHazardRate*AN40)-EXP(-QuantoHazardRate*AN41))</f>
+        <f t="shared" si="31"/>
         <v>-</v>
       </c>
       <c r="AS41" s="23" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>-</v>
       </c>
       <c r="AT41" s="22" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>-</v>
       </c>
       <c r="AU41" s="25" t="str">
@@ -23726,7 +23726,7 @@
     <row r="42" spans="8:47">
       <c r="P42" s="3"/>
       <c r="R42" s="35">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>10</v>
       </c>
       <c r="S42" s="22" t="str">
@@ -23766,39 +23766,39 @@
         <v>-</v>
       </c>
       <c r="AC42" s="21">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>10</v>
       </c>
       <c r="AD42" s="22" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>-</v>
       </c>
       <c r="AE42" s="24" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>-</v>
       </c>
       <c r="AF42" s="41" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>-</v>
       </c>
       <c r="AG42" s="22" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>-</v>
       </c>
       <c r="AH42" s="23" t="str">
-        <f>IF(AC42&gt;Maturity,"-",EXP(-DomesticHazardRate*AC41)-EXP(-DomesticHazardRate*AC42))</f>
+        <f t="shared" si="27"/>
         <v>-</v>
       </c>
       <c r="AI42" s="23" t="str">
-        <f>IF(AC42&gt;Maturity,"-",EXP(-QuantoHazardRate*AC41)-EXP(-QuantoHazardRate*AC42))</f>
+        <f t="shared" si="28"/>
         <v>-</v>
       </c>
       <c r="AJ42" s="23" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>-</v>
       </c>
       <c r="AK42" s="22" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>-</v>
       </c>
       <c r="AL42" s="25" t="str">
@@ -23806,31 +23806,31 @@
         <v>-</v>
       </c>
       <c r="AN42" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>10</v>
       </c>
       <c r="AO42" s="22" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>-</v>
       </c>
       <c r="AP42" s="22" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>-</v>
       </c>
       <c r="AQ42" s="23" t="str">
-        <f>IF(AN42&gt;Maturity,"-",EXP(-DomesticHazardRate*AN41)-EXP(-DomesticHazardRate*AN42))</f>
+        <f t="shared" si="30"/>
         <v>-</v>
       </c>
       <c r="AR42" s="23" t="str">
-        <f>IF(AN42&gt;Maturity,"-",EXP(-QuantoHazardRate*AN41)-EXP(-QuantoHazardRate*AN42))</f>
+        <f t="shared" si="31"/>
         <v>-</v>
       </c>
       <c r="AS42" s="23" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>-</v>
       </c>
       <c r="AT42" s="22" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>-</v>
       </c>
       <c r="AU42" s="25" t="str">
@@ -23841,7 +23841,7 @@
     <row r="43" spans="8:47">
       <c r="P43" s="3"/>
       <c r="R43" s="35">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>10.25</v>
       </c>
       <c r="S43" s="22" t="str">
@@ -23881,39 +23881,39 @@
         <v>-</v>
       </c>
       <c r="AC43" s="21">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>10.25</v>
       </c>
       <c r="AD43" s="22" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>-</v>
       </c>
       <c r="AE43" s="24" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>-</v>
       </c>
       <c r="AF43" s="41" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>-</v>
       </c>
       <c r="AG43" s="22" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>-</v>
       </c>
       <c r="AH43" s="23" t="str">
-        <f>IF(AC43&gt;Maturity,"-",EXP(-DomesticHazardRate*AC42)-EXP(-DomesticHazardRate*AC43))</f>
+        <f t="shared" si="27"/>
         <v>-</v>
       </c>
       <c r="AI43" s="23" t="str">
-        <f>IF(AC43&gt;Maturity,"-",EXP(-QuantoHazardRate*AC42)-EXP(-QuantoHazardRate*AC43))</f>
+        <f t="shared" si="28"/>
         <v>-</v>
       </c>
       <c r="AJ43" s="23" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>-</v>
       </c>
       <c r="AK43" s="22" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>-</v>
       </c>
       <c r="AL43" s="25" t="str">
@@ -23921,31 +23921,31 @@
         <v>-</v>
       </c>
       <c r="AN43" s="21">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>10.25</v>
       </c>
       <c r="AO43" s="22" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>-</v>
       </c>
       <c r="AP43" s="22" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>-</v>
       </c>
       <c r="AQ43" s="23" t="str">
-        <f>IF(AN43&gt;Maturity,"-",EXP(-DomesticHazardRate*AN42)-EXP(-DomesticHazardRate*AN43))</f>
+        <f t="shared" si="30"/>
         <v>-</v>
       </c>
       <c r="AR43" s="23" t="str">
-        <f>IF(AN43&gt;Maturity,"-",EXP(-QuantoHazardRate*AN42)-EXP(-QuantoHazardRate*AN43))</f>
+        <f t="shared" si="31"/>
         <v>-</v>
       </c>
       <c r="AS43" s="23" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>-</v>
       </c>
       <c r="AT43" s="22" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>-</v>
       </c>
       <c r="AU43" s="25" t="str">
@@ -23956,7 +23956,7 @@
     <row r="44" spans="8:47">
       <c r="P44" s="3"/>
       <c r="R44" s="37">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>10.5</v>
       </c>
       <c r="S44" s="27" t="str">
@@ -23996,39 +23996,39 @@
         <v>-</v>
       </c>
       <c r="AC44" s="26">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>10.5</v>
       </c>
       <c r="AD44" s="27" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>-</v>
       </c>
       <c r="AE44" s="29" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>-</v>
       </c>
       <c r="AF44" s="42" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>-</v>
       </c>
       <c r="AG44" s="27" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>-</v>
       </c>
       <c r="AH44" s="28" t="str">
-        <f>IF(AC44&gt;Maturity,"-",EXP(-DomesticHazardRate*AC43)-EXP(-DomesticHazardRate*AC44))</f>
+        <f t="shared" si="27"/>
         <v>-</v>
       </c>
       <c r="AI44" s="28" t="str">
-        <f>IF(AC44&gt;Maturity,"-",EXP(-QuantoHazardRate*AC43)-EXP(-QuantoHazardRate*AC44))</f>
+        <f t="shared" si="28"/>
         <v>-</v>
       </c>
       <c r="AJ44" s="28" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>-</v>
       </c>
       <c r="AK44" s="27" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>-</v>
       </c>
       <c r="AL44" s="30" t="str">
@@ -24036,31 +24036,31 @@
         <v>-</v>
       </c>
       <c r="AN44" s="26">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>10.5</v>
       </c>
       <c r="AO44" s="27" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>-</v>
       </c>
       <c r="AP44" s="27" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>-</v>
       </c>
       <c r="AQ44" s="28" t="str">
-        <f>IF(AN44&gt;Maturity,"-",EXP(-DomesticHazardRate*AN43)-EXP(-DomesticHazardRate*AN44))</f>
+        <f t="shared" si="30"/>
         <v>-</v>
       </c>
       <c r="AR44" s="28" t="str">
-        <f>IF(AN44&gt;Maturity,"-",EXP(-QuantoHazardRate*AN43)-EXP(-QuantoHazardRate*AN44))</f>
+        <f t="shared" si="31"/>
         <v>-</v>
       </c>
       <c r="AS44" s="28" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>-</v>
       </c>
       <c r="AT44" s="27" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>-</v>
       </c>
       <c r="AU44" s="30" t="str">
@@ -24094,7 +24094,7 @@
       </c>
       <c r="AA47" s="43">
         <f>SUM(AA3:AA44)</f>
-        <v>-66793.950186463466</v>
+        <v>-66747.344094916145</v>
       </c>
       <c r="AK47" s="43">
         <f>SUM(AK3:AK44)</f>
@@ -24102,7 +24102,7 @@
       </c>
       <c r="AL47" s="43">
         <f>SUM(AL3:AL44)</f>
-        <v>-277.28979001241635</v>
+        <v>-279.5949708295467</v>
       </c>
       <c r="AT47" s="43">
         <f>SUM(AT3:AT44)</f>
@@ -24110,7 +24110,7 @@
       </c>
       <c r="AU47" s="43">
         <f>SUM(AU3:AU44)</f>
-        <v>71558.655487075201</v>
+        <v>72153.540859237866</v>
       </c>
     </row>
     <row r="48" spans="8:47">

</xml_diff>